<commit_message>
Add DEBUG BreakPoint to GUI. Support TestingProgram1.
</commit_message>
<xml_diff>
--- a/TestProgram1(Assembly-Code).xlsx
+++ b/TestProgram1(Assembly-Code).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QiTianYi\Desktop\Advanced Computer Architecture\CSCI6461ComputerArchitecture\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88F5849D-6B7B-4F2C-87BF-07AD28FCF01A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AFB049A-52CC-4C7C-9962-0E65ED4A7B9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-7110" yWindow="5025" windowWidth="14400" windowHeight="7875" xr2:uid="{5181C135-F803-4CA6-AFB1-3DD996B2224A}"/>
+    <workbookView xWindow="-6765" yWindow="4755" windowWidth="14400" windowHeight="7875" xr2:uid="{5181C135-F803-4CA6-AFB1-3DD996B2224A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="136">
   <si>
     <t>Memory Location</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -366,10 +366,6 @@
   </si>
   <si>
     <t>JMA IX0,14 (AFTER THE INSTR, THE SPACE USE AS SWAP)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RESULT AT MEM[29]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -541,6 +537,90 @@
   </si>
   <si>
     <t>JSR IX0,22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,MEM[29]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDA R2,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DVD R0,R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[20]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R2,MEM[20]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R2,MEM[19]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIR R2,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R2,MEM[19]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMR R2,MEM[19]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R1,IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNE R0,IX0,24</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,MEM[20]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMR R0,MEM[19]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R0,MEM[20]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>READ NUMBER REVERSE ORDER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>OUT R0,PRINTER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,MEM[19]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R0,MEM[19]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMA IX0,23</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[18]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -843,7 +923,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -925,9 +1005,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
@@ -937,13 +1014,19 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -952,8 +1035,29 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -973,34 +1077,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1">
+      <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -1320,8 +1403,8 @@
   <dimension ref="A1:R1026"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
-      <pane ySplit="33" topLeftCell="A193" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G26" sqref="G26"/>
+      <pane ySplit="33" topLeftCell="A241" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C8" sqref="C8:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1339,7 +1422,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="2" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
@@ -1349,12 +1432,12 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="49" t="s">
+      <c r="C2" s="31" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1363,10 +1446,10 @@
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="49"/>
-      <c r="D3" s="49"/>
-      <c r="E3" s="49"/>
-      <c r="F3" s="49"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
     </row>
     <row r="4" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
@@ -1375,10 +1458,10 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="49"/>
-      <c r="D4" s="49"/>
-      <c r="E4" s="49"/>
-      <c r="F4" s="49"/>
+      <c r="C4" s="31"/>
+      <c r="D4" s="31"/>
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
     </row>
     <row r="5" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
@@ -1387,10 +1470,10 @@
       <c r="B5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C5" s="49"/>
-      <c r="D5" s="49"/>
-      <c r="E5" s="49"/>
-      <c r="F5" s="49"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
     </row>
     <row r="6" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -1399,10 +1482,10 @@
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="49"/>
-      <c r="D6" s="49"/>
-      <c r="E6" s="49"/>
-      <c r="F6" s="49"/>
+      <c r="C6" s="31"/>
+      <c r="D6" s="31"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
     </row>
     <row r="7" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
@@ -1411,10 +1494,10 @@
       <c r="B7" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="49"/>
-      <c r="D7" s="49"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+      <c r="E7" s="31"/>
+      <c r="F7" s="31"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -1423,12 +1506,12 @@
       <c r="B8" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="C8" s="50" t="s">
+      <c r="C8" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
@@ -1437,144 +1520,150 @@
       <c r="B9" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C9" s="51"/>
-      <c r="D9" s="51"/>
-      <c r="E9" s="51"/>
-      <c r="F9" s="51"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+    </row>
+    <row r="10" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="51"/>
-      <c r="D10" s="51"/>
-      <c r="E10" s="51"/>
-      <c r="F10" s="51"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+        <v>86</v>
+      </c>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+    </row>
+    <row r="11" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="C11" s="51"/>
-      <c r="D11" s="51"/>
-      <c r="E11" s="51"/>
-      <c r="F11" s="51"/>
+        <v>87</v>
+      </c>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
+      <c r="F11" s="33"/>
     </row>
     <row r="12" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="51"/>
-      <c r="D12" s="51"/>
-      <c r="E12" s="51"/>
-      <c r="F12" s="51"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
+      <c r="F12" s="33"/>
     </row>
     <row r="13" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="51"/>
-      <c r="D13" s="51"/>
-      <c r="E13" s="51"/>
-      <c r="F13" s="51"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="51"/>
-      <c r="D14" s="51"/>
-      <c r="E14" s="51"/>
-      <c r="F14" s="51"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
+      <c r="F14" s="33"/>
     </row>
     <row r="15" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="13"/>
-      <c r="C15" s="51"/>
-      <c r="D15" s="51"/>
-      <c r="E15" s="51"/>
-      <c r="F15" s="51"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
     </row>
     <row r="16" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="13"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="51"/>
-      <c r="E16" s="51"/>
-      <c r="F16" s="51"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
+      <c r="F16" s="33"/>
     </row>
     <row r="17" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="51"/>
-      <c r="E17" s="51"/>
-      <c r="F17" s="51"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
+      <c r="F17" s="33"/>
     </row>
     <row r="18" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="51"/>
-      <c r="E18" s="51"/>
-      <c r="F18" s="51"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
+      <c r="F18" s="33"/>
     </row>
     <row r="19" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="13"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="51"/>
-      <c r="E19" s="51"/>
-      <c r="F19" s="51"/>
-    </row>
-    <row r="20" spans="1:6" hidden="1" x14ac:dyDescent="0.2">
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
+      <c r="F19" s="33"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
-      <c r="B20" s="14"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="51"/>
-      <c r="E20" s="51"/>
-      <c r="F20" s="51"/>
+      <c r="B20" s="14">
+        <v>251</v>
+      </c>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
+      <c r="F20" s="33"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
-      <c r="B21" s="3"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="51"/>
-      <c r="E21" s="51"/>
-      <c r="F21" s="51"/>
+      <c r="B21" s="3">
+        <v>0</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
-      <c r="B22" s="3"/>
-      <c r="C22" s="51"/>
-      <c r="D22" s="51"/>
-      <c r="E22" s="51"/>
-      <c r="F22" s="51"/>
+      <c r="B22" s="3">
+        <v>1000</v>
+      </c>
+      <c r="C22" s="33"/>
+      <c r="D22" s="33"/>
+      <c r="E22" s="33"/>
+      <c r="F22" s="33"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
@@ -1583,10 +1672,10 @@
       <c r="B23" s="3">
         <v>210</v>
       </c>
-      <c r="C23" s="51"/>
-      <c r="D23" s="51"/>
-      <c r="E23" s="51"/>
-      <c r="F23" s="51"/>
+      <c r="C23" s="33"/>
+      <c r="D23" s="33"/>
+      <c r="E23" s="33"/>
+      <c r="F23" s="33"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
@@ -1595,10 +1684,10 @@
       <c r="B24" s="3">
         <v>177</v>
       </c>
-      <c r="C24" s="51"/>
-      <c r="D24" s="51"/>
-      <c r="E24" s="51"/>
-      <c r="F24" s="51"/>
+      <c r="C24" s="33"/>
+      <c r="D24" s="33"/>
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
@@ -1607,22 +1696,22 @@
       <c r="B25" s="3">
         <v>65535</v>
       </c>
-      <c r="C25" s="51"/>
-      <c r="D25" s="51"/>
-      <c r="E25" s="51"/>
-      <c r="F25" s="51"/>
+      <c r="C25" s="33"/>
+      <c r="D25" s="33"/>
+      <c r="E25" s="33"/>
+      <c r="F25" s="33"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A26" s="52">
+      <c r="A26" s="30">
         <v>24</v>
       </c>
-      <c r="B26" s="52">
+      <c r="B26" s="30">
         <v>145</v>
       </c>
-      <c r="C26" s="51"/>
-      <c r="D26" s="51"/>
-      <c r="E26" s="51"/>
-      <c r="F26" s="51"/>
+      <c r="C26" s="33"/>
+      <c r="D26" s="33"/>
+      <c r="E26" s="33"/>
+      <c r="F26" s="33"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
@@ -1631,10 +1720,10 @@
       <c r="B27" s="3">
         <v>105</v>
       </c>
-      <c r="C27" s="51"/>
-      <c r="D27" s="51"/>
-      <c r="E27" s="51"/>
-      <c r="F27" s="51"/>
+      <c r="C27" s="33"/>
+      <c r="D27" s="33"/>
+      <c r="E27" s="33"/>
+      <c r="F27" s="33"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
@@ -1643,22 +1732,22 @@
       <c r="B28" s="3">
         <v>500</v>
       </c>
-      <c r="C28" s="51"/>
-      <c r="D28" s="51"/>
-      <c r="E28" s="51"/>
-      <c r="F28" s="51"/>
+      <c r="C28" s="33"/>
+      <c r="D28" s="33"/>
+      <c r="E28" s="33"/>
+      <c r="F28" s="33"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A29" s="52">
+      <c r="A29" s="30">
         <v>27</v>
       </c>
-      <c r="B29" s="52">
+      <c r="B29" s="30">
         <v>20</v>
       </c>
-      <c r="C29" s="51"/>
-      <c r="D29" s="51"/>
-      <c r="E29" s="51"/>
-      <c r="F29" s="51"/>
+      <c r="C29" s="33"/>
+      <c r="D29" s="33"/>
+      <c r="E29" s="33"/>
+      <c r="F29" s="33"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
@@ -1667,10 +1756,10 @@
       <c r="B30" s="3">
         <v>67</v>
       </c>
-      <c r="C30" s="51"/>
-      <c r="D30" s="51"/>
-      <c r="E30" s="51"/>
-      <c r="F30" s="51"/>
+      <c r="C30" s="33"/>
+      <c r="D30" s="33"/>
+      <c r="E30" s="33"/>
+      <c r="F30" s="33"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
@@ -1679,10 +1768,10 @@
       <c r="B31" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="51"/>
-      <c r="D31" s="51"/>
-      <c r="E31" s="51"/>
-      <c r="F31" s="51"/>
+      <c r="C31" s="33"/>
+      <c r="D31" s="33"/>
+      <c r="E31" s="33"/>
+      <c r="F31" s="33"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
@@ -1691,10 +1780,10 @@
       <c r="B32" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="C32" s="51"/>
-      <c r="D32" s="51"/>
-      <c r="E32" s="51"/>
-      <c r="F32" s="51"/>
+      <c r="C32" s="33"/>
+      <c r="D32" s="33"/>
+      <c r="E32" s="33"/>
+      <c r="F32" s="33"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -1703,10 +1792,10 @@
       <c r="B33" s="5">
         <v>32</v>
       </c>
-      <c r="C33" s="51"/>
-      <c r="D33" s="51"/>
-      <c r="E33" s="51"/>
-      <c r="F33" s="51"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="33"/>
+      <c r="E33" s="33"/>
+      <c r="F33" s="33"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -1715,14 +1804,14 @@
       <c r="B34" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C34" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" s="36" t="s">
-        <v>90</v>
-      </c>
-      <c r="E34" s="36"/>
-      <c r="F34" s="44"/>
+      <c r="C34" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D34" s="38" t="s">
+        <v>89</v>
+      </c>
+      <c r="E34" s="38"/>
+      <c r="F34" s="39"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -1731,10 +1820,10 @@
       <c r="B35" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="45"/>
-      <c r="E35" s="45"/>
-      <c r="F35" s="46"/>
+      <c r="C35" s="35"/>
+      <c r="D35" s="40"/>
+      <c r="E35" s="40"/>
+      <c r="F35" s="41"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -1743,10 +1832,10 @@
       <c r="B36" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="45"/>
-      <c r="E36" s="45"/>
-      <c r="F36" s="46"/>
+      <c r="C36" s="35"/>
+      <c r="D36" s="40"/>
+      <c r="E36" s="40"/>
+      <c r="F36" s="41"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -1755,10 +1844,10 @@
       <c r="B37" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="45"/>
-      <c r="E37" s="45"/>
-      <c r="F37" s="46"/>
+      <c r="C37" s="35"/>
+      <c r="D37" s="40"/>
+      <c r="E37" s="40"/>
+      <c r="F37" s="41"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
@@ -1767,10 +1856,10 @@
       <c r="B38" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C38" s="34"/>
-      <c r="D38" s="45"/>
-      <c r="E38" s="45"/>
-      <c r="F38" s="46"/>
+      <c r="C38" s="35"/>
+      <c r="D38" s="40"/>
+      <c r="E38" s="40"/>
+      <c r="F38" s="41"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
@@ -1779,22 +1868,22 @@
       <c r="B39" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="34"/>
-      <c r="D39" s="45"/>
-      <c r="E39" s="45"/>
-      <c r="F39" s="46"/>
+      <c r="C39" s="35"/>
+      <c r="D39" s="40"/>
+      <c r="E39" s="40"/>
+      <c r="F39" s="41"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A40" s="29">
+      <c r="A40" s="28">
         <v>38</v>
       </c>
-      <c r="B40" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C40" s="34"/>
-      <c r="D40" s="45"/>
-      <c r="E40" s="45"/>
-      <c r="F40" s="46"/>
+      <c r="B40" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C40" s="35"/>
+      <c r="D40" s="40"/>
+      <c r="E40" s="40"/>
+      <c r="F40" s="41"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -1803,10 +1892,10 @@
       <c r="B41" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C41" s="35"/>
-      <c r="D41" s="45"/>
-      <c r="E41" s="45"/>
-      <c r="F41" s="46"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="40"/>
+      <c r="F41" s="41"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -1816,9 +1905,9 @@
         <v>12</v>
       </c>
       <c r="C42" s="17"/>
-      <c r="D42" s="45"/>
-      <c r="E42" s="45"/>
-      <c r="F42" s="46"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="40"/>
+      <c r="F42" s="41"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -1828,9 +1917,9 @@
         <v>13</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="45"/>
-      <c r="E43" s="45"/>
-      <c r="F43" s="46"/>
+      <c r="D43" s="40"/>
+      <c r="E43" s="40"/>
+      <c r="F43" s="41"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -1840,9 +1929,9 @@
         <v>11</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="45"/>
-      <c r="E44" s="45"/>
-      <c r="F44" s="46"/>
+      <c r="D44" s="40"/>
+      <c r="E44" s="40"/>
+      <c r="F44" s="41"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -1852,9 +1941,9 @@
         <v>37</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="45"/>
-      <c r="E45" s="45"/>
-      <c r="F45" s="46"/>
+      <c r="D45" s="40"/>
+      <c r="E45" s="40"/>
+      <c r="F45" s="41"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -1864,9 +1953,9 @@
         <v>9</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="45"/>
-      <c r="E46" s="45"/>
-      <c r="F46" s="46"/>
+      <c r="D46" s="40"/>
+      <c r="E46" s="40"/>
+      <c r="F46" s="41"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -1876,9 +1965,9 @@
         <v>14</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="45"/>
-      <c r="E47" s="45"/>
-      <c r="F47" s="46"/>
+      <c r="D47" s="40"/>
+      <c r="E47" s="40"/>
+      <c r="F47" s="41"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -1888,9 +1977,9 @@
         <v>38</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="45"/>
-      <c r="E48" s="45"/>
-      <c r="F48" s="46"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="40"/>
+      <c r="F48" s="41"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -1900,9 +1989,9 @@
         <v>17</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="D49" s="45"/>
-      <c r="E49" s="45"/>
-      <c r="F49" s="46"/>
+      <c r="D49" s="40"/>
+      <c r="E49" s="40"/>
+      <c r="F49" s="41"/>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -1912,9 +2001,9 @@
         <v>18</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="45"/>
-      <c r="E50" s="45"/>
-      <c r="F50" s="46"/>
+      <c r="D50" s="40"/>
+      <c r="E50" s="40"/>
+      <c r="F50" s="41"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -1924,9 +2013,9 @@
         <v>19</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="45"/>
-      <c r="E51" s="45"/>
-      <c r="F51" s="46"/>
+      <c r="D51" s="40"/>
+      <c r="E51" s="40"/>
+      <c r="F51" s="41"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -1935,12 +2024,12 @@
       <c r="B52" s="18" t="s">
         <v>34</v>
       </c>
-      <c r="C52" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D52" s="45"/>
-      <c r="E52" s="45"/>
-      <c r="F52" s="46"/>
+      <c r="C52" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D52" s="40"/>
+      <c r="E52" s="40"/>
+      <c r="F52" s="41"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -1949,10 +2038,10 @@
       <c r="B53" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C53" s="34"/>
-      <c r="D53" s="45"/>
-      <c r="E53" s="45"/>
-      <c r="F53" s="46"/>
+      <c r="C53" s="35"/>
+      <c r="D53" s="40"/>
+      <c r="E53" s="40"/>
+      <c r="F53" s="41"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -1961,10 +2050,10 @@
       <c r="B54" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C54" s="34"/>
-      <c r="D54" s="45"/>
-      <c r="E54" s="45"/>
-      <c r="F54" s="46"/>
+      <c r="C54" s="35"/>
+      <c r="D54" s="40"/>
+      <c r="E54" s="40"/>
+      <c r="F54" s="41"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -1973,10 +2062,10 @@
       <c r="B55" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C55" s="34"/>
-      <c r="D55" s="45"/>
-      <c r="E55" s="45"/>
-      <c r="F55" s="46"/>
+      <c r="C55" s="35"/>
+      <c r="D55" s="40"/>
+      <c r="E55" s="40"/>
+      <c r="F55" s="41"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -1985,10 +2074,10 @@
       <c r="B56" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C56" s="34"/>
-      <c r="D56" s="45"/>
-      <c r="E56" s="45"/>
-      <c r="F56" s="46"/>
+      <c r="C56" s="35"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="40"/>
+      <c r="F56" s="41"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -1997,10 +2086,10 @@
       <c r="B57" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C57" s="34"/>
-      <c r="D57" s="45"/>
-      <c r="E57" s="45"/>
-      <c r="F57" s="46"/>
+      <c r="C57" s="35"/>
+      <c r="D57" s="40"/>
+      <c r="E57" s="40"/>
+      <c r="F57" s="41"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -2009,10 +2098,10 @@
       <c r="B58" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C58" s="34"/>
-      <c r="D58" s="45"/>
-      <c r="E58" s="45"/>
-      <c r="F58" s="46"/>
+      <c r="C58" s="35"/>
+      <c r="D58" s="40"/>
+      <c r="E58" s="40"/>
+      <c r="F58" s="41"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -2021,10 +2110,10 @@
       <c r="B59" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C59" s="35"/>
-      <c r="D59" s="45"/>
-      <c r="E59" s="45"/>
-      <c r="F59" s="46"/>
+      <c r="C59" s="36"/>
+      <c r="D59" s="40"/>
+      <c r="E59" s="40"/>
+      <c r="F59" s="41"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -2034,9 +2123,9 @@
         <v>10</v>
       </c>
       <c r="C60" s="9"/>
-      <c r="D60" s="47"/>
-      <c r="E60" s="47"/>
-      <c r="F60" s="48"/>
+      <c r="D60" s="42"/>
+      <c r="E60" s="42"/>
+      <c r="F60" s="43"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
@@ -2045,14 +2134,14 @@
       <c r="B61" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C61" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="D61" s="36" t="s">
-        <v>91</v>
-      </c>
-      <c r="E61" s="37"/>
-      <c r="F61" s="38"/>
+      <c r="C61" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D61" s="38" t="s">
+        <v>90</v>
+      </c>
+      <c r="E61" s="45"/>
+      <c r="F61" s="46"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -2061,10 +2150,10 @@
       <c r="B62" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C62" s="34"/>
-      <c r="D62" s="39"/>
-      <c r="E62" s="39"/>
-      <c r="F62" s="40"/>
+      <c r="C62" s="35"/>
+      <c r="D62" s="47"/>
+      <c r="E62" s="47"/>
+      <c r="F62" s="48"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -2073,10 +2162,10 @@
       <c r="B63" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C63" s="34"/>
-      <c r="D63" s="39"/>
-      <c r="E63" s="39"/>
-      <c r="F63" s="40"/>
+      <c r="C63" s="35"/>
+      <c r="D63" s="47"/>
+      <c r="E63" s="47"/>
+      <c r="F63" s="48"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
@@ -2085,10 +2174,10 @@
       <c r="B64" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C64" s="34"/>
-      <c r="D64" s="39"/>
-      <c r="E64" s="39"/>
-      <c r="F64" s="40"/>
+      <c r="C64" s="35"/>
+      <c r="D64" s="47"/>
+      <c r="E64" s="47"/>
+      <c r="F64" s="48"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -2097,10 +2186,10 @@
       <c r="B65" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C65" s="34"/>
-      <c r="D65" s="39"/>
-      <c r="E65" s="39"/>
-      <c r="F65" s="40"/>
+      <c r="C65" s="35"/>
+      <c r="D65" s="47"/>
+      <c r="E65" s="47"/>
+      <c r="F65" s="48"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -2109,22 +2198,22 @@
       <c r="B66" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C66" s="34"/>
-      <c r="D66" s="39"/>
-      <c r="E66" s="39"/>
-      <c r="F66" s="40"/>
+      <c r="C66" s="35"/>
+      <c r="D66" s="47"/>
+      <c r="E66" s="47"/>
+      <c r="F66" s="48"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="29">
+      <c r="A67" s="28">
         <v>65</v>
       </c>
-      <c r="B67" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C67" s="34"/>
-      <c r="D67" s="39"/>
-      <c r="E67" s="39"/>
-      <c r="F67" s="40"/>
+      <c r="B67" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C67" s="35"/>
+      <c r="D67" s="47"/>
+      <c r="E67" s="47"/>
+      <c r="F67" s="48"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -2133,10 +2222,10 @@
       <c r="B68" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C68" s="35"/>
-      <c r="D68" s="39"/>
-      <c r="E68" s="39"/>
-      <c r="F68" s="40"/>
+      <c r="C68" s="36"/>
+      <c r="D68" s="47"/>
+      <c r="E68" s="47"/>
+      <c r="F68" s="48"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
@@ -2146,21 +2235,21 @@
         <v>15</v>
       </c>
       <c r="C69" s="7"/>
-      <c r="D69" s="39"/>
-      <c r="E69" s="39"/>
-      <c r="F69" s="40"/>
+      <c r="D69" s="47"/>
+      <c r="E69" s="47"/>
+      <c r="F69" s="48"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="C70" s="7"/>
-      <c r="D70" s="39"/>
-      <c r="E70" s="39"/>
-      <c r="F70" s="40"/>
+      <c r="D70" s="47"/>
+      <c r="E70" s="47"/>
+      <c r="F70" s="48"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -2170,9 +2259,9 @@
         <v>11</v>
       </c>
       <c r="C71" s="7"/>
-      <c r="D71" s="39"/>
-      <c r="E71" s="39"/>
-      <c r="F71" s="40"/>
+      <c r="D71" s="47"/>
+      <c r="E71" s="47"/>
+      <c r="F71" s="48"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -2182,9 +2271,9 @@
         <v>8</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="39"/>
-      <c r="E72" s="39"/>
-      <c r="F72" s="40"/>
+      <c r="D72" s="47"/>
+      <c r="E72" s="47"/>
+      <c r="F72" s="48"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="15">
@@ -2194,9 +2283,9 @@
         <v>41</v>
       </c>
       <c r="C73" s="7"/>
-      <c r="D73" s="39"/>
-      <c r="E73" s="39"/>
-      <c r="F73" s="40"/>
+      <c r="D73" s="47"/>
+      <c r="E73" s="47"/>
+      <c r="F73" s="48"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -2206,9 +2295,9 @@
         <v>16</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="39"/>
-      <c r="E74" s="39"/>
-      <c r="F74" s="40"/>
+      <c r="D74" s="47"/>
+      <c r="E74" s="47"/>
+      <c r="F74" s="48"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -2218,9 +2307,9 @@
         <v>12</v>
       </c>
       <c r="C75" s="7"/>
-      <c r="D75" s="39"/>
-      <c r="E75" s="39"/>
-      <c r="F75" s="40"/>
+      <c r="D75" s="47"/>
+      <c r="E75" s="47"/>
+      <c r="F75" s="48"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2230,9 +2319,9 @@
         <v>13</v>
       </c>
       <c r="C76" s="7"/>
-      <c r="D76" s="39"/>
-      <c r="E76" s="39"/>
-      <c r="F76" s="40"/>
+      <c r="D76" s="47"/>
+      <c r="E76" s="47"/>
+      <c r="F76" s="48"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -2242,9 +2331,9 @@
         <v>21</v>
       </c>
       <c r="C77" s="7"/>
-      <c r="D77" s="39"/>
-      <c r="E77" s="39"/>
-      <c r="F77" s="40"/>
+      <c r="D77" s="47"/>
+      <c r="E77" s="47"/>
+      <c r="F77" s="48"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="2">
@@ -2254,21 +2343,21 @@
         <v>15</v>
       </c>
       <c r="C78" s="7"/>
-      <c r="D78" s="39"/>
-      <c r="E78" s="39"/>
-      <c r="F78" s="40"/>
+      <c r="D78" s="47"/>
+      <c r="E78" s="47"/>
+      <c r="F78" s="48"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C79" s="7"/>
-      <c r="D79" s="39"/>
-      <c r="E79" s="39"/>
-      <c r="F79" s="40"/>
+      <c r="D79" s="47"/>
+      <c r="E79" s="47"/>
+      <c r="F79" s="48"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -2278,9 +2367,9 @@
         <v>8</v>
       </c>
       <c r="C80" s="7"/>
-      <c r="D80" s="39"/>
-      <c r="E80" s="39"/>
-      <c r="F80" s="40"/>
+      <c r="D80" s="47"/>
+      <c r="E80" s="47"/>
+      <c r="F80" s="48"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
@@ -2290,9 +2379,9 @@
         <v>29</v>
       </c>
       <c r="C81" s="7"/>
-      <c r="D81" s="39"/>
-      <c r="E81" s="39"/>
-      <c r="F81" s="40"/>
+      <c r="D81" s="47"/>
+      <c r="E81" s="47"/>
+      <c r="F81" s="48"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
@@ -2302,9 +2391,9 @@
         <v>44</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="39"/>
-      <c r="E82" s="39"/>
-      <c r="F82" s="40"/>
+      <c r="D82" s="47"/>
+      <c r="E82" s="47"/>
+      <c r="F82" s="48"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
@@ -2314,9 +2403,9 @@
         <v>11</v>
       </c>
       <c r="C83" s="7"/>
-      <c r="D83" s="39"/>
-      <c r="E83" s="39"/>
-      <c r="F83" s="40"/>
+      <c r="D83" s="47"/>
+      <c r="E83" s="47"/>
+      <c r="F83" s="48"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
@@ -2326,9 +2415,9 @@
         <v>16</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="39"/>
-      <c r="E84" s="39"/>
-      <c r="F84" s="40"/>
+      <c r="D84" s="47"/>
+      <c r="E84" s="47"/>
+      <c r="F84" s="48"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
@@ -2338,9 +2427,9 @@
         <v>12</v>
       </c>
       <c r="C85" s="7"/>
-      <c r="D85" s="39"/>
-      <c r="E85" s="39"/>
-      <c r="F85" s="40"/>
+      <c r="D85" s="47"/>
+      <c r="E85" s="47"/>
+      <c r="F85" s="48"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
@@ -2350,9 +2439,9 @@
         <v>13</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="39"/>
-      <c r="E86" s="39"/>
-      <c r="F86" s="40"/>
+      <c r="D86" s="47"/>
+      <c r="E86" s="47"/>
+      <c r="F86" s="48"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
@@ -2362,9 +2451,9 @@
         <v>25</v>
       </c>
       <c r="C87" s="7"/>
-      <c r="D87" s="39"/>
-      <c r="E87" s="39"/>
-      <c r="F87" s="40"/>
+      <c r="D87" s="47"/>
+      <c r="E87" s="47"/>
+      <c r="F87" s="48"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
@@ -2374,9 +2463,9 @@
         <v>22</v>
       </c>
       <c r="C88" s="7"/>
-      <c r="D88" s="39"/>
-      <c r="E88" s="39"/>
-      <c r="F88" s="40"/>
+      <c r="D88" s="47"/>
+      <c r="E88" s="47"/>
+      <c r="F88" s="48"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
@@ -2386,9 +2475,9 @@
         <v>23</v>
       </c>
       <c r="C89" s="7"/>
-      <c r="D89" s="39"/>
-      <c r="E89" s="39"/>
-      <c r="F89" s="40"/>
+      <c r="D89" s="47"/>
+      <c r="E89" s="47"/>
+      <c r="F89" s="48"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -2398,9 +2487,9 @@
         <v>24</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="39"/>
-      <c r="E90" s="39"/>
-      <c r="F90" s="40"/>
+      <c r="D90" s="47"/>
+      <c r="E90" s="47"/>
+      <c r="F90" s="48"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -2410,9 +2499,9 @@
         <v>11</v>
       </c>
       <c r="C91" s="7"/>
-      <c r="D91" s="39"/>
-      <c r="E91" s="39"/>
-      <c r="F91" s="40"/>
+      <c r="D91" s="47"/>
+      <c r="E91" s="47"/>
+      <c r="F91" s="48"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
@@ -2422,9 +2511,9 @@
         <v>42</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="39"/>
-      <c r="E92" s="39"/>
-      <c r="F92" s="40"/>
+      <c r="D92" s="47"/>
+      <c r="E92" s="47"/>
+      <c r="F92" s="48"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -2434,9 +2523,9 @@
         <v>28</v>
       </c>
       <c r="C93" s="7"/>
-      <c r="D93" s="39"/>
-      <c r="E93" s="39"/>
-      <c r="F93" s="40"/>
+      <c r="D93" s="47"/>
+      <c r="E93" s="47"/>
+      <c r="F93" s="48"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -2446,9 +2535,9 @@
         <v>43</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="39"/>
-      <c r="E94" s="39"/>
-      <c r="F94" s="40"/>
+      <c r="D94" s="47"/>
+      <c r="E94" s="47"/>
+      <c r="F94" s="48"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
@@ -2458,9 +2547,9 @@
         <v>21</v>
       </c>
       <c r="C95" s="7"/>
-      <c r="D95" s="39"/>
-      <c r="E95" s="39"/>
-      <c r="F95" s="40"/>
+      <c r="D95" s="47"/>
+      <c r="E95" s="47"/>
+      <c r="F95" s="48"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -2470,21 +2559,21 @@
         <v>29</v>
       </c>
       <c r="C96" s="7"/>
-      <c r="D96" s="39"/>
-      <c r="E96" s="39"/>
-      <c r="F96" s="40"/>
+      <c r="D96" s="47"/>
+      <c r="E96" s="47"/>
+      <c r="F96" s="48"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C97" s="7"/>
-      <c r="D97" s="39"/>
-      <c r="E97" s="39"/>
-      <c r="F97" s="40"/>
+      <c r="D97" s="47"/>
+      <c r="E97" s="47"/>
+      <c r="F97" s="48"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
@@ -2493,12 +2582,12 @@
       <c r="B98" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="C98" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D98" s="39"/>
-      <c r="E98" s="39"/>
-      <c r="F98" s="40"/>
+      <c r="C98" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D98" s="47"/>
+      <c r="E98" s="47"/>
+      <c r="F98" s="48"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
@@ -2507,10 +2596,10 @@
       <c r="B99" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C99" s="34"/>
-      <c r="D99" s="39"/>
-      <c r="E99" s="39"/>
-      <c r="F99" s="40"/>
+      <c r="C99" s="35"/>
+      <c r="D99" s="47"/>
+      <c r="E99" s="47"/>
+      <c r="F99" s="48"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
@@ -2519,10 +2608,10 @@
       <c r="B100" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C100" s="34"/>
-      <c r="D100" s="39"/>
-      <c r="E100" s="39"/>
-      <c r="F100" s="40"/>
+      <c r="C100" s="35"/>
+      <c r="D100" s="47"/>
+      <c r="E100" s="47"/>
+      <c r="F100" s="48"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
@@ -2531,10 +2620,10 @@
       <c r="B101" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C101" s="34"/>
-      <c r="D101" s="39"/>
-      <c r="E101" s="39"/>
-      <c r="F101" s="40"/>
+      <c r="C101" s="35"/>
+      <c r="D101" s="47"/>
+      <c r="E101" s="47"/>
+      <c r="F101" s="48"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
@@ -2543,10 +2632,10 @@
       <c r="B102" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C102" s="34"/>
-      <c r="D102" s="39"/>
-      <c r="E102" s="39"/>
-      <c r="F102" s="40"/>
+      <c r="C102" s="35"/>
+      <c r="D102" s="47"/>
+      <c r="E102" s="47"/>
+      <c r="F102" s="48"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
@@ -2555,10 +2644,10 @@
       <c r="B103" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C103" s="34"/>
-      <c r="D103" s="39"/>
-      <c r="E103" s="39"/>
-      <c r="F103" s="40"/>
+      <c r="C103" s="35"/>
+      <c r="D103" s="47"/>
+      <c r="E103" s="47"/>
+      <c r="F103" s="48"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -2567,10 +2656,10 @@
       <c r="B104" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C104" s="34"/>
-      <c r="D104" s="39"/>
-      <c r="E104" s="39"/>
-      <c r="F104" s="40"/>
+      <c r="C104" s="35"/>
+      <c r="D104" s="47"/>
+      <c r="E104" s="47"/>
+      <c r="F104" s="48"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
@@ -2579,10 +2668,10 @@
       <c r="B105" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C105" s="35"/>
-      <c r="D105" s="39"/>
-      <c r="E105" s="39"/>
-      <c r="F105" s="40"/>
+      <c r="C105" s="36"/>
+      <c r="D105" s="47"/>
+      <c r="E105" s="47"/>
+      <c r="F105" s="48"/>
     </row>
     <row r="106" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -2592,9 +2681,9 @@
         <v>10</v>
       </c>
       <c r="C106" s="9"/>
-      <c r="D106" s="41"/>
-      <c r="E106" s="41"/>
-      <c r="F106" s="42"/>
+      <c r="D106" s="49"/>
+      <c r="E106" s="49"/>
+      <c r="F106" s="50"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
@@ -2603,14 +2692,14 @@
       <c r="B107" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C107" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="D107" s="36" t="s">
-        <v>92</v>
-      </c>
-      <c r="E107" s="37"/>
-      <c r="F107" s="38"/>
+      <c r="C107" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D107" s="38" t="s">
+        <v>91</v>
+      </c>
+      <c r="E107" s="45"/>
+      <c r="F107" s="46"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
@@ -2619,10 +2708,10 @@
       <c r="B108" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C108" s="34"/>
-      <c r="D108" s="39"/>
-      <c r="E108" s="39"/>
-      <c r="F108" s="40"/>
+      <c r="C108" s="35"/>
+      <c r="D108" s="47"/>
+      <c r="E108" s="47"/>
+      <c r="F108" s="48"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -2631,10 +2720,10 @@
       <c r="B109" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C109" s="34"/>
-      <c r="D109" s="39"/>
-      <c r="E109" s="39"/>
-      <c r="F109" s="40"/>
+      <c r="C109" s="35"/>
+      <c r="D109" s="47"/>
+      <c r="E109" s="47"/>
+      <c r="F109" s="48"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -2643,10 +2732,10 @@
       <c r="B110" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C110" s="34"/>
-      <c r="D110" s="39"/>
-      <c r="E110" s="39"/>
-      <c r="F110" s="40"/>
+      <c r="C110" s="35"/>
+      <c r="D110" s="47"/>
+      <c r="E110" s="47"/>
+      <c r="F110" s="48"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
@@ -2655,10 +2744,10 @@
       <c r="B111" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C111" s="34"/>
-      <c r="D111" s="39"/>
-      <c r="E111" s="39"/>
-      <c r="F111" s="40"/>
+      <c r="C111" s="35"/>
+      <c r="D111" s="47"/>
+      <c r="E111" s="47"/>
+      <c r="F111" s="48"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
@@ -2667,22 +2756,22 @@
       <c r="B112" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C112" s="34"/>
-      <c r="D112" s="39"/>
-      <c r="E112" s="39"/>
-      <c r="F112" s="40"/>
+      <c r="C112" s="35"/>
+      <c r="D112" s="47"/>
+      <c r="E112" s="47"/>
+      <c r="F112" s="48"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A113" s="29">
+      <c r="A113" s="28">
         <v>111</v>
       </c>
-      <c r="B113" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C113" s="34"/>
-      <c r="D113" s="39"/>
-      <c r="E113" s="39"/>
-      <c r="F113" s="40"/>
+      <c r="B113" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C113" s="35"/>
+      <c r="D113" s="47"/>
+      <c r="E113" s="47"/>
+      <c r="F113" s="48"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
@@ -2691,10 +2780,10 @@
       <c r="B114" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C114" s="35"/>
-      <c r="D114" s="39"/>
-      <c r="E114" s="39"/>
-      <c r="F114" s="40"/>
+      <c r="C114" s="36"/>
+      <c r="D114" s="47"/>
+      <c r="E114" s="47"/>
+      <c r="F114" s="48"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
@@ -2704,9 +2793,9 @@
         <v>11</v>
       </c>
       <c r="C115" s="7"/>
-      <c r="D115" s="39"/>
-      <c r="E115" s="39"/>
-      <c r="F115" s="40"/>
+      <c r="D115" s="47"/>
+      <c r="E115" s="47"/>
+      <c r="F115" s="48"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
@@ -2716,9 +2805,9 @@
         <v>45</v>
       </c>
       <c r="C116" s="7"/>
-      <c r="D116" s="39"/>
-      <c r="E116" s="39"/>
-      <c r="F116" s="40"/>
+      <c r="D116" s="47"/>
+      <c r="E116" s="47"/>
+      <c r="F116" s="48"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
@@ -2728,9 +2817,9 @@
         <v>46</v>
       </c>
       <c r="C117" s="7"/>
-      <c r="D117" s="39"/>
-      <c r="E117" s="39"/>
-      <c r="F117" s="40"/>
+      <c r="D117" s="47"/>
+      <c r="E117" s="47"/>
+      <c r="F117" s="48"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
@@ -2740,9 +2829,9 @@
         <v>47</v>
       </c>
       <c r="C118" s="7"/>
-      <c r="D118" s="39"/>
-      <c r="E118" s="39"/>
-      <c r="F118" s="40"/>
+      <c r="D118" s="47"/>
+      <c r="E118" s="47"/>
+      <c r="F118" s="48"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
@@ -2752,9 +2841,9 @@
         <v>32</v>
       </c>
       <c r="C119" s="7"/>
-      <c r="D119" s="39"/>
-      <c r="E119" s="39"/>
-      <c r="F119" s="40"/>
+      <c r="D119" s="47"/>
+      <c r="E119" s="47"/>
+      <c r="F119" s="48"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
@@ -2764,9 +2853,9 @@
         <v>48</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="39"/>
-      <c r="E120" s="39"/>
-      <c r="F120" s="40"/>
+      <c r="D120" s="47"/>
+      <c r="E120" s="47"/>
+      <c r="F120" s="48"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
@@ -2776,9 +2865,9 @@
         <v>22</v>
       </c>
       <c r="C121" s="7"/>
-      <c r="D121" s="39"/>
-      <c r="E121" s="39"/>
-      <c r="F121" s="40"/>
+      <c r="D121" s="47"/>
+      <c r="E121" s="47"/>
+      <c r="F121" s="48"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
@@ -2788,9 +2877,9 @@
         <v>49</v>
       </c>
       <c r="C122" s="7"/>
-      <c r="D122" s="39"/>
-      <c r="E122" s="39"/>
-      <c r="F122" s="40"/>
+      <c r="D122" s="47"/>
+      <c r="E122" s="47"/>
+      <c r="F122" s="48"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
@@ -2800,9 +2889,9 @@
         <v>46</v>
       </c>
       <c r="C123" s="7"/>
-      <c r="D123" s="39"/>
-      <c r="E123" s="39"/>
-      <c r="F123" s="40"/>
+      <c r="D123" s="47"/>
+      <c r="E123" s="47"/>
+      <c r="F123" s="48"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
@@ -2812,9 +2901,9 @@
         <v>40</v>
       </c>
       <c r="C124" s="7"/>
-      <c r="D124" s="39"/>
-      <c r="E124" s="39"/>
-      <c r="F124" s="40"/>
+      <c r="D124" s="47"/>
+      <c r="E124" s="47"/>
+      <c r="F124" s="48"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
@@ -2824,9 +2913,9 @@
         <v>50</v>
       </c>
       <c r="C125" s="7"/>
-      <c r="D125" s="39"/>
-      <c r="E125" s="39"/>
-      <c r="F125" s="40"/>
+      <c r="D125" s="47"/>
+      <c r="E125" s="47"/>
+      <c r="F125" s="48"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
@@ -2836,21 +2925,21 @@
         <v>51</v>
       </c>
       <c r="C126" s="7"/>
-      <c r="D126" s="39"/>
-      <c r="E126" s="39"/>
-      <c r="F126" s="40"/>
+      <c r="D126" s="47"/>
+      <c r="E126" s="47"/>
+      <c r="F126" s="48"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C127" s="7"/>
-      <c r="D127" s="39"/>
-      <c r="E127" s="39"/>
-      <c r="F127" s="40"/>
+      <c r="D127" s="47"/>
+      <c r="E127" s="47"/>
+      <c r="F127" s="48"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="15">
@@ -2859,12 +2948,12 @@
       <c r="B128" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C128" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D128" s="39"/>
-      <c r="E128" s="39"/>
-      <c r="F128" s="40"/>
+      <c r="C128" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D128" s="47"/>
+      <c r="E128" s="47"/>
+      <c r="F128" s="48"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
@@ -2873,10 +2962,10 @@
       <c r="B129" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C129" s="34"/>
-      <c r="D129" s="39"/>
-      <c r="E129" s="39"/>
-      <c r="F129" s="40"/>
+      <c r="C129" s="35"/>
+      <c r="D129" s="47"/>
+      <c r="E129" s="47"/>
+      <c r="F129" s="48"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
@@ -2885,10 +2974,10 @@
       <c r="B130" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C130" s="34"/>
-      <c r="D130" s="39"/>
-      <c r="E130" s="39"/>
-      <c r="F130" s="40"/>
+      <c r="C130" s="35"/>
+      <c r="D130" s="47"/>
+      <c r="E130" s="47"/>
+      <c r="F130" s="48"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
@@ -2897,10 +2986,10 @@
       <c r="B131" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C131" s="34"/>
-      <c r="D131" s="39"/>
-      <c r="E131" s="39"/>
-      <c r="F131" s="40"/>
+      <c r="C131" s="35"/>
+      <c r="D131" s="47"/>
+      <c r="E131" s="47"/>
+      <c r="F131" s="48"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
@@ -2909,10 +2998,10 @@
       <c r="B132" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C132" s="34"/>
-      <c r="D132" s="39"/>
-      <c r="E132" s="39"/>
-      <c r="F132" s="40"/>
+      <c r="C132" s="35"/>
+      <c r="D132" s="47"/>
+      <c r="E132" s="47"/>
+      <c r="F132" s="48"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
@@ -2921,10 +3010,10 @@
       <c r="B133" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C133" s="34"/>
-      <c r="D133" s="39"/>
-      <c r="E133" s="39"/>
-      <c r="F133" s="40"/>
+      <c r="C133" s="35"/>
+      <c r="D133" s="47"/>
+      <c r="E133" s="47"/>
+      <c r="F133" s="48"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
@@ -2933,10 +3022,10 @@
       <c r="B134" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C134" s="34"/>
-      <c r="D134" s="39"/>
-      <c r="E134" s="39"/>
-      <c r="F134" s="40"/>
+      <c r="C134" s="35"/>
+      <c r="D134" s="47"/>
+      <c r="E134" s="47"/>
+      <c r="F134" s="48"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
@@ -2945,10 +3034,10 @@
       <c r="B135" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C135" s="35"/>
-      <c r="D135" s="39"/>
-      <c r="E135" s="39"/>
-      <c r="F135" s="40"/>
+      <c r="C135" s="36"/>
+      <c r="D135" s="47"/>
+      <c r="E135" s="47"/>
+      <c r="F135" s="48"/>
     </row>
     <row r="136" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -2958,9 +3047,9 @@
         <v>10</v>
       </c>
       <c r="C136" s="7"/>
-      <c r="D136" s="39"/>
-      <c r="E136" s="39"/>
-      <c r="F136" s="40"/>
+      <c r="D136" s="47"/>
+      <c r="E136" s="47"/>
+      <c r="F136" s="48"/>
     </row>
     <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
@@ -2969,14 +3058,14 @@
       <c r="B137" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C137" s="43" t="s">
-        <v>86</v>
-      </c>
-      <c r="D137" s="36" t="s">
-        <v>96</v>
-      </c>
-      <c r="E137" s="36"/>
-      <c r="F137" s="44"/>
+      <c r="C137" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D137" s="38" t="s">
+        <v>95</v>
+      </c>
+      <c r="E137" s="38"/>
+      <c r="F137" s="39"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
@@ -2985,10 +3074,10 @@
       <c r="B138" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C138" s="34"/>
-      <c r="D138" s="45"/>
-      <c r="E138" s="45"/>
-      <c r="F138" s="46"/>
+      <c r="C138" s="35"/>
+      <c r="D138" s="40"/>
+      <c r="E138" s="40"/>
+      <c r="F138" s="41"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
@@ -2997,10 +3086,10 @@
       <c r="B139" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C139" s="34"/>
-      <c r="D139" s="45"/>
-      <c r="E139" s="45"/>
-      <c r="F139" s="46"/>
+      <c r="C139" s="35"/>
+      <c r="D139" s="40"/>
+      <c r="E139" s="40"/>
+      <c r="F139" s="41"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
@@ -3009,10 +3098,10 @@
       <c r="B140" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C140" s="34"/>
-      <c r="D140" s="45"/>
-      <c r="E140" s="45"/>
-      <c r="F140" s="46"/>
+      <c r="C140" s="35"/>
+      <c r="D140" s="40"/>
+      <c r="E140" s="40"/>
+      <c r="F140" s="41"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
@@ -3021,10 +3110,10 @@
       <c r="B141" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C141" s="34"/>
-      <c r="D141" s="45"/>
-      <c r="E141" s="45"/>
-      <c r="F141" s="46"/>
+      <c r="C141" s="35"/>
+      <c r="D141" s="40"/>
+      <c r="E141" s="40"/>
+      <c r="F141" s="41"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
@@ -3033,22 +3122,22 @@
       <c r="B142" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C142" s="34"/>
-      <c r="D142" s="45"/>
-      <c r="E142" s="45"/>
-      <c r="F142" s="46"/>
+      <c r="C142" s="35"/>
+      <c r="D142" s="40"/>
+      <c r="E142" s="40"/>
+      <c r="F142" s="41"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A143" s="29">
+      <c r="A143" s="28">
         <v>141</v>
       </c>
-      <c r="B143" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C143" s="34"/>
-      <c r="D143" s="45"/>
-      <c r="E143" s="45"/>
-      <c r="F143" s="46"/>
+      <c r="B143" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C143" s="35"/>
+      <c r="D143" s="40"/>
+      <c r="E143" s="40"/>
+      <c r="F143" s="41"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
@@ -3057,10 +3146,10 @@
       <c r="B144" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C144" s="35"/>
-      <c r="D144" s="45"/>
-      <c r="E144" s="45"/>
-      <c r="F144" s="46"/>
+      <c r="C144" s="36"/>
+      <c r="D144" s="40"/>
+      <c r="E144" s="40"/>
+      <c r="F144" s="41"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
@@ -3070,9 +3159,9 @@
         <v>52</v>
       </c>
       <c r="C145" s="7"/>
-      <c r="D145" s="45"/>
-      <c r="E145" s="45"/>
-      <c r="F145" s="46"/>
+      <c r="D145" s="40"/>
+      <c r="E145" s="40"/>
+      <c r="F145" s="41"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
@@ -3082,9 +3171,9 @@
         <v>53</v>
       </c>
       <c r="C146" s="7"/>
-      <c r="D146" s="45"/>
-      <c r="E146" s="45"/>
-      <c r="F146" s="46"/>
+      <c r="D146" s="40"/>
+      <c r="E146" s="40"/>
+      <c r="F146" s="41"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
@@ -3094,9 +3183,9 @@
         <v>57</v>
       </c>
       <c r="C147" s="7"/>
-      <c r="D147" s="45"/>
-      <c r="E147" s="45"/>
-      <c r="F147" s="46"/>
+      <c r="D147" s="40"/>
+      <c r="E147" s="40"/>
+      <c r="F147" s="41"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
@@ -3106,9 +3195,9 @@
         <v>58</v>
       </c>
       <c r="C148" s="7"/>
-      <c r="D148" s="45"/>
-      <c r="E148" s="45"/>
-      <c r="F148" s="46"/>
+      <c r="D148" s="40"/>
+      <c r="E148" s="40"/>
+      <c r="F148" s="41"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
@@ -3118,11 +3207,11 @@
         <v>56</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D149" s="45"/>
-      <c r="E149" s="45"/>
-      <c r="F149" s="46"/>
+        <v>92</v>
+      </c>
+      <c r="D149" s="40"/>
+      <c r="E149" s="40"/>
+      <c r="F149" s="41"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
@@ -3131,12 +3220,12 @@
       <c r="B150" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C150" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D150" s="45"/>
-      <c r="E150" s="45"/>
-      <c r="F150" s="46"/>
+      <c r="C150" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D150" s="40"/>
+      <c r="E150" s="40"/>
+      <c r="F150" s="41"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
@@ -3145,10 +3234,10 @@
       <c r="B151" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C151" s="34"/>
-      <c r="D151" s="45"/>
-      <c r="E151" s="45"/>
-      <c r="F151" s="46"/>
+      <c r="C151" s="35"/>
+      <c r="D151" s="40"/>
+      <c r="E151" s="40"/>
+      <c r="F151" s="41"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
@@ -3157,10 +3246,10 @@
       <c r="B152" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C152" s="34"/>
-      <c r="D152" s="45"/>
-      <c r="E152" s="45"/>
-      <c r="F152" s="46"/>
+      <c r="C152" s="35"/>
+      <c r="D152" s="40"/>
+      <c r="E152" s="40"/>
+      <c r="F152" s="41"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
@@ -3169,10 +3258,10 @@
       <c r="B153" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C153" s="34"/>
-      <c r="D153" s="45"/>
-      <c r="E153" s="45"/>
-      <c r="F153" s="46"/>
+      <c r="C153" s="35"/>
+      <c r="D153" s="40"/>
+      <c r="E153" s="40"/>
+      <c r="F153" s="41"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
@@ -3181,10 +3270,10 @@
       <c r="B154" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C154" s="34"/>
-      <c r="D154" s="45"/>
-      <c r="E154" s="45"/>
-      <c r="F154" s="46"/>
+      <c r="C154" s="35"/>
+      <c r="D154" s="40"/>
+      <c r="E154" s="40"/>
+      <c r="F154" s="41"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
@@ -3193,10 +3282,10 @@
       <c r="B155" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C155" s="34"/>
-      <c r="D155" s="45"/>
-      <c r="E155" s="45"/>
-      <c r="F155" s="46"/>
+      <c r="C155" s="35"/>
+      <c r="D155" s="40"/>
+      <c r="E155" s="40"/>
+      <c r="F155" s="41"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
@@ -3205,10 +3294,10 @@
       <c r="B156" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C156" s="34"/>
-      <c r="D156" s="45"/>
-      <c r="E156" s="45"/>
-      <c r="F156" s="46"/>
+      <c r="C156" s="35"/>
+      <c r="D156" s="40"/>
+      <c r="E156" s="40"/>
+      <c r="F156" s="41"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
@@ -3217,10 +3306,10 @@
       <c r="B157" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C157" s="35"/>
-      <c r="D157" s="45"/>
-      <c r="E157" s="45"/>
-      <c r="F157" s="46"/>
+      <c r="C157" s="36"/>
+      <c r="D157" s="40"/>
+      <c r="E157" s="40"/>
+      <c r="F157" s="41"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="15">
@@ -3230,11 +3319,11 @@
         <v>54</v>
       </c>
       <c r="C158" s="25" t="s">
-        <v>94</v>
-      </c>
-      <c r="D158" s="45"/>
-      <c r="E158" s="45"/>
-      <c r="F158" s="46"/>
+        <v>93</v>
+      </c>
+      <c r="D158" s="40"/>
+      <c r="E158" s="40"/>
+      <c r="F158" s="41"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
@@ -3244,11 +3333,11 @@
         <v>56</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="D159" s="45"/>
-      <c r="E159" s="45"/>
-      <c r="F159" s="46"/>
+        <v>92</v>
+      </c>
+      <c r="D159" s="40"/>
+      <c r="E159" s="40"/>
+      <c r="F159" s="41"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
@@ -3257,12 +3346,12 @@
       <c r="B160" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C160" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D160" s="45"/>
-      <c r="E160" s="45"/>
-      <c r="F160" s="46"/>
+      <c r="C160" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D160" s="40"/>
+      <c r="E160" s="40"/>
+      <c r="F160" s="41"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
@@ -3271,10 +3360,10 @@
       <c r="B161" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C161" s="34"/>
-      <c r="D161" s="45"/>
-      <c r="E161" s="45"/>
-      <c r="F161" s="46"/>
+      <c r="C161" s="35"/>
+      <c r="D161" s="40"/>
+      <c r="E161" s="40"/>
+      <c r="F161" s="41"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
@@ -3283,10 +3372,10 @@
       <c r="B162" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C162" s="34"/>
-      <c r="D162" s="45"/>
-      <c r="E162" s="45"/>
-      <c r="F162" s="46"/>
+      <c r="C162" s="35"/>
+      <c r="D162" s="40"/>
+      <c r="E162" s="40"/>
+      <c r="F162" s="41"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
@@ -3295,10 +3384,10 @@
       <c r="B163" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C163" s="34"/>
-      <c r="D163" s="45"/>
-      <c r="E163" s="45"/>
-      <c r="F163" s="46"/>
+      <c r="C163" s="35"/>
+      <c r="D163" s="40"/>
+      <c r="E163" s="40"/>
+      <c r="F163" s="41"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
@@ -3307,10 +3396,10 @@
       <c r="B164" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C164" s="34"/>
-      <c r="D164" s="45"/>
-      <c r="E164" s="45"/>
-      <c r="F164" s="46"/>
+      <c r="C164" s="35"/>
+      <c r="D164" s="40"/>
+      <c r="E164" s="40"/>
+      <c r="F164" s="41"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
@@ -3319,10 +3408,10 @@
       <c r="B165" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C165" s="34"/>
-      <c r="D165" s="45"/>
-      <c r="E165" s="45"/>
-      <c r="F165" s="46"/>
+      <c r="C165" s="35"/>
+      <c r="D165" s="40"/>
+      <c r="E165" s="40"/>
+      <c r="F165" s="41"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
@@ -3331,10 +3420,10 @@
       <c r="B166" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C166" s="34"/>
-      <c r="D166" s="45"/>
-      <c r="E166" s="45"/>
-      <c r="F166" s="46"/>
+      <c r="C166" s="35"/>
+      <c r="D166" s="40"/>
+      <c r="E166" s="40"/>
+      <c r="F166" s="41"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
@@ -3343,10 +3432,10 @@
       <c r="B167" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C167" s="35"/>
-      <c r="D167" s="45"/>
-      <c r="E167" s="45"/>
-      <c r="F167" s="46"/>
+      <c r="C167" s="36"/>
+      <c r="D167" s="40"/>
+      <c r="E167" s="40"/>
+      <c r="F167" s="41"/>
     </row>
     <row r="168" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
@@ -3356,11 +3445,11 @@
         <v>55</v>
       </c>
       <c r="C168" s="26" t="s">
-        <v>95</v>
-      </c>
-      <c r="D168" s="47"/>
-      <c r="E168" s="47"/>
-      <c r="F168" s="48"/>
+        <v>94</v>
+      </c>
+      <c r="D168" s="42"/>
+      <c r="E168" s="42"/>
+      <c r="F168" s="43"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
@@ -3369,14 +3458,14 @@
       <c r="B169" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="C169" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D169" s="36" t="s">
-        <v>97</v>
-      </c>
-      <c r="E169" s="37"/>
-      <c r="F169" s="38"/>
+      <c r="C169" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D169" s="38" t="s">
+        <v>96</v>
+      </c>
+      <c r="E169" s="45"/>
+      <c r="F169" s="46"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
@@ -3385,10 +3474,10 @@
       <c r="B170" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C170" s="34"/>
-      <c r="D170" s="39"/>
-      <c r="E170" s="39"/>
-      <c r="F170" s="40"/>
+      <c r="C170" s="35"/>
+      <c r="D170" s="47"/>
+      <c r="E170" s="47"/>
+      <c r="F170" s="48"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
@@ -3397,10 +3486,10 @@
       <c r="B171" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C171" s="34"/>
-      <c r="D171" s="39"/>
-      <c r="E171" s="39"/>
-      <c r="F171" s="40"/>
+      <c r="C171" s="35"/>
+      <c r="D171" s="47"/>
+      <c r="E171" s="47"/>
+      <c r="F171" s="48"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
@@ -3409,10 +3498,10 @@
       <c r="B172" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C172" s="34"/>
-      <c r="D172" s="39"/>
-      <c r="E172" s="39"/>
-      <c r="F172" s="40"/>
+      <c r="C172" s="35"/>
+      <c r="D172" s="47"/>
+      <c r="E172" s="47"/>
+      <c r="F172" s="48"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
@@ -3421,10 +3510,10 @@
       <c r="B173" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C173" s="34"/>
-      <c r="D173" s="39"/>
-      <c r="E173" s="39"/>
-      <c r="F173" s="40"/>
+      <c r="C173" s="35"/>
+      <c r="D173" s="47"/>
+      <c r="E173" s="47"/>
+      <c r="F173" s="48"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
@@ -3433,22 +3522,22 @@
       <c r="B174" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C174" s="34"/>
-      <c r="D174" s="39"/>
-      <c r="E174" s="39"/>
-      <c r="F174" s="40"/>
+      <c r="C174" s="35"/>
+      <c r="D174" s="47"/>
+      <c r="E174" s="47"/>
+      <c r="F174" s="48"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A175" s="29">
+      <c r="A175" s="28">
         <v>173</v>
       </c>
-      <c r="B175" s="30" t="s">
-        <v>110</v>
-      </c>
-      <c r="C175" s="34"/>
-      <c r="D175" s="39"/>
-      <c r="E175" s="39"/>
-      <c r="F175" s="40"/>
+      <c r="B175" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="C175" s="35"/>
+      <c r="D175" s="47"/>
+      <c r="E175" s="47"/>
+      <c r="F175" s="48"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
@@ -3457,10 +3546,10 @@
       <c r="B176" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="C176" s="35"/>
-      <c r="D176" s="39"/>
-      <c r="E176" s="39"/>
-      <c r="F176" s="40"/>
+      <c r="C176" s="36"/>
+      <c r="D176" s="47"/>
+      <c r="E176" s="47"/>
+      <c r="F176" s="48"/>
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
@@ -3470,22 +3559,22 @@
         <v>60</v>
       </c>
       <c r="C177" s="7"/>
-      <c r="D177" s="39"/>
-      <c r="E177" s="39"/>
-      <c r="F177" s="40"/>
-      <c r="H177" s="31" t="s">
-        <v>107</v>
-      </c>
-      <c r="I177" s="32"/>
-      <c r="J177" s="32"/>
-      <c r="K177" s="32"/>
-      <c r="L177" s="32"/>
-      <c r="M177" s="32"/>
-      <c r="N177" s="32"/>
-      <c r="O177" s="32"/>
-      <c r="P177" s="32"/>
-      <c r="Q177" s="32"/>
-      <c r="R177" s="32"/>
+      <c r="D177" s="47"/>
+      <c r="E177" s="47"/>
+      <c r="F177" s="48"/>
+      <c r="H177" s="51" t="s">
+        <v>106</v>
+      </c>
+      <c r="I177" s="44"/>
+      <c r="J177" s="44"/>
+      <c r="K177" s="44"/>
+      <c r="L177" s="44"/>
+      <c r="M177" s="44"/>
+      <c r="N177" s="44"/>
+      <c r="O177" s="44"/>
+      <c r="P177" s="44"/>
+      <c r="Q177" s="44"/>
+      <c r="R177" s="44"/>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
@@ -3495,20 +3584,20 @@
         <v>50</v>
       </c>
       <c r="C178" s="7"/>
-      <c r="D178" s="39"/>
-      <c r="E178" s="39"/>
-      <c r="F178" s="40"/>
-      <c r="H178" s="32"/>
-      <c r="I178" s="32"/>
-      <c r="J178" s="32"/>
-      <c r="K178" s="32"/>
-      <c r="L178" s="32"/>
-      <c r="M178" s="32"/>
-      <c r="N178" s="32"/>
-      <c r="O178" s="32"/>
-      <c r="P178" s="32"/>
-      <c r="Q178" s="32"/>
-      <c r="R178" s="32"/>
+      <c r="D178" s="47"/>
+      <c r="E178" s="47"/>
+      <c r="F178" s="48"/>
+      <c r="H178" s="44"/>
+      <c r="I178" s="44"/>
+      <c r="J178" s="44"/>
+      <c r="K178" s="44"/>
+      <c r="L178" s="44"/>
+      <c r="M178" s="44"/>
+      <c r="N178" s="44"/>
+      <c r="O178" s="44"/>
+      <c r="P178" s="44"/>
+      <c r="Q178" s="44"/>
+      <c r="R178" s="44"/>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
@@ -3518,22 +3607,22 @@
         <v>61</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="D179" s="39"/>
-      <c r="E179" s="39"/>
-      <c r="F179" s="40"/>
-      <c r="H179" s="32"/>
-      <c r="I179" s="32"/>
-      <c r="J179" s="32"/>
-      <c r="K179" s="32"/>
-      <c r="L179" s="32"/>
-      <c r="M179" s="32"/>
-      <c r="N179" s="32"/>
-      <c r="O179" s="32"/>
-      <c r="P179" s="32"/>
-      <c r="Q179" s="32"/>
-      <c r="R179" s="32"/>
+        <v>97</v>
+      </c>
+      <c r="D179" s="47"/>
+      <c r="E179" s="47"/>
+      <c r="F179" s="48"/>
+      <c r="H179" s="44"/>
+      <c r="I179" s="44"/>
+      <c r="J179" s="44"/>
+      <c r="K179" s="44"/>
+      <c r="L179" s="44"/>
+      <c r="M179" s="44"/>
+      <c r="N179" s="44"/>
+      <c r="O179" s="44"/>
+      <c r="P179" s="44"/>
+      <c r="Q179" s="44"/>
+      <c r="R179" s="44"/>
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
@@ -3543,20 +3632,20 @@
         <v>62</v>
       </c>
       <c r="C180" s="7"/>
-      <c r="D180" s="39"/>
-      <c r="E180" s="39"/>
-      <c r="F180" s="40"/>
-      <c r="H180" s="32"/>
-      <c r="I180" s="32"/>
-      <c r="J180" s="32"/>
-      <c r="K180" s="32"/>
-      <c r="L180" s="32"/>
-      <c r="M180" s="32"/>
-      <c r="N180" s="32"/>
-      <c r="O180" s="32"/>
-      <c r="P180" s="32"/>
-      <c r="Q180" s="32"/>
-      <c r="R180" s="32"/>
+      <c r="D180" s="47"/>
+      <c r="E180" s="47"/>
+      <c r="F180" s="48"/>
+      <c r="H180" s="44"/>
+      <c r="I180" s="44"/>
+      <c r="J180" s="44"/>
+      <c r="K180" s="44"/>
+      <c r="L180" s="44"/>
+      <c r="M180" s="44"/>
+      <c r="N180" s="44"/>
+      <c r="O180" s="44"/>
+      <c r="P180" s="44"/>
+      <c r="Q180" s="44"/>
+      <c r="R180" s="44"/>
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
@@ -3566,20 +3655,20 @@
         <v>32</v>
       </c>
       <c r="C181" s="7"/>
-      <c r="D181" s="39"/>
-      <c r="E181" s="39"/>
-      <c r="F181" s="40"/>
-      <c r="H181" s="32"/>
-      <c r="I181" s="32"/>
-      <c r="J181" s="32"/>
-      <c r="K181" s="32"/>
-      <c r="L181" s="32"/>
-      <c r="M181" s="32"/>
-      <c r="N181" s="32"/>
-      <c r="O181" s="32"/>
-      <c r="P181" s="32"/>
-      <c r="Q181" s="32"/>
-      <c r="R181" s="32"/>
+      <c r="D181" s="47"/>
+      <c r="E181" s="47"/>
+      <c r="F181" s="48"/>
+      <c r="H181" s="44"/>
+      <c r="I181" s="44"/>
+      <c r="J181" s="44"/>
+      <c r="K181" s="44"/>
+      <c r="L181" s="44"/>
+      <c r="M181" s="44"/>
+      <c r="N181" s="44"/>
+      <c r="O181" s="44"/>
+      <c r="P181" s="44"/>
+      <c r="Q181" s="44"/>
+      <c r="R181" s="44"/>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
@@ -3589,20 +3678,20 @@
         <v>48</v>
       </c>
       <c r="C182" s="7"/>
-      <c r="D182" s="39"/>
-      <c r="E182" s="39"/>
-      <c r="F182" s="40"/>
-      <c r="H182" s="32"/>
-      <c r="I182" s="32"/>
-      <c r="J182" s="32"/>
-      <c r="K182" s="32"/>
-      <c r="L182" s="32"/>
-      <c r="M182" s="32"/>
-      <c r="N182" s="32"/>
-      <c r="O182" s="32"/>
-      <c r="P182" s="32"/>
-      <c r="Q182" s="32"/>
-      <c r="R182" s="32"/>
+      <c r="D182" s="47"/>
+      <c r="E182" s="47"/>
+      <c r="F182" s="48"/>
+      <c r="H182" s="44"/>
+      <c r="I182" s="44"/>
+      <c r="J182" s="44"/>
+      <c r="K182" s="44"/>
+      <c r="L182" s="44"/>
+      <c r="M182" s="44"/>
+      <c r="N182" s="44"/>
+      <c r="O182" s="44"/>
+      <c r="P182" s="44"/>
+      <c r="Q182" s="44"/>
+      <c r="R182" s="44"/>
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
@@ -3614,20 +3703,20 @@
       <c r="C183" s="7" t="s">
         <v>64</v>
       </c>
-      <c r="D183" s="39"/>
-      <c r="E183" s="39"/>
-      <c r="F183" s="40"/>
-      <c r="H183" s="32"/>
-      <c r="I183" s="32"/>
-      <c r="J183" s="32"/>
-      <c r="K183" s="32"/>
-      <c r="L183" s="32"/>
-      <c r="M183" s="32"/>
-      <c r="N183" s="32"/>
-      <c r="O183" s="32"/>
-      <c r="P183" s="32"/>
-      <c r="Q183" s="32"/>
-      <c r="R183" s="32"/>
+      <c r="D183" s="47"/>
+      <c r="E183" s="47"/>
+      <c r="F183" s="48"/>
+      <c r="H183" s="44"/>
+      <c r="I183" s="44"/>
+      <c r="J183" s="44"/>
+      <c r="K183" s="44"/>
+      <c r="L183" s="44"/>
+      <c r="M183" s="44"/>
+      <c r="N183" s="44"/>
+      <c r="O183" s="44"/>
+      <c r="P183" s="44"/>
+      <c r="Q183" s="44"/>
+      <c r="R183" s="44"/>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
@@ -3637,22 +3726,22 @@
         <v>65</v>
       </c>
       <c r="C184" s="7" t="s">
-        <v>103</v>
-      </c>
-      <c r="D184" s="39"/>
-      <c r="E184" s="39"/>
-      <c r="F184" s="40"/>
-      <c r="H184" s="32"/>
-      <c r="I184" s="32"/>
-      <c r="J184" s="32"/>
-      <c r="K184" s="32"/>
-      <c r="L184" s="32"/>
-      <c r="M184" s="32"/>
-      <c r="N184" s="32"/>
-      <c r="O184" s="32"/>
-      <c r="P184" s="32"/>
-      <c r="Q184" s="32"/>
-      <c r="R184" s="32"/>
+        <v>102</v>
+      </c>
+      <c r="D184" s="47"/>
+      <c r="E184" s="47"/>
+      <c r="F184" s="48"/>
+      <c r="H184" s="44"/>
+      <c r="I184" s="44"/>
+      <c r="J184" s="44"/>
+      <c r="K184" s="44"/>
+      <c r="L184" s="44"/>
+      <c r="M184" s="44"/>
+      <c r="N184" s="44"/>
+      <c r="O184" s="44"/>
+      <c r="P184" s="44"/>
+      <c r="Q184" s="44"/>
+      <c r="R184" s="44"/>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
@@ -3662,20 +3751,20 @@
         <v>51</v>
       </c>
       <c r="C185" s="7"/>
-      <c r="D185" s="39"/>
-      <c r="E185" s="39"/>
-      <c r="F185" s="40"/>
-      <c r="H185" s="32"/>
-      <c r="I185" s="32"/>
-      <c r="J185" s="32"/>
-      <c r="K185" s="32"/>
-      <c r="L185" s="32"/>
-      <c r="M185" s="32"/>
-      <c r="N185" s="32"/>
-      <c r="O185" s="32"/>
-      <c r="P185" s="32"/>
-      <c r="Q185" s="32"/>
-      <c r="R185" s="32"/>
+      <c r="D185" s="47"/>
+      <c r="E185" s="47"/>
+      <c r="F185" s="48"/>
+      <c r="H185" s="44"/>
+      <c r="I185" s="44"/>
+      <c r="J185" s="44"/>
+      <c r="K185" s="44"/>
+      <c r="L185" s="44"/>
+      <c r="M185" s="44"/>
+      <c r="N185" s="44"/>
+      <c r="O185" s="44"/>
+      <c r="P185" s="44"/>
+      <c r="Q185" s="44"/>
+      <c r="R185" s="44"/>
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
@@ -3685,22 +3774,22 @@
         <v>66</v>
       </c>
       <c r="C186" s="7" t="s">
-        <v>102</v>
-      </c>
-      <c r="D186" s="39"/>
-      <c r="E186" s="39"/>
-      <c r="F186" s="40"/>
-      <c r="H186" s="32"/>
-      <c r="I186" s="32"/>
-      <c r="J186" s="32"/>
-      <c r="K186" s="32"/>
-      <c r="L186" s="32"/>
-      <c r="M186" s="32"/>
-      <c r="N186" s="32"/>
-      <c r="O186" s="32"/>
-      <c r="P186" s="32"/>
-      <c r="Q186" s="32"/>
-      <c r="R186" s="32"/>
+        <v>101</v>
+      </c>
+      <c r="D186" s="47"/>
+      <c r="E186" s="47"/>
+      <c r="F186" s="48"/>
+      <c r="H186" s="44"/>
+      <c r="I186" s="44"/>
+      <c r="J186" s="44"/>
+      <c r="K186" s="44"/>
+      <c r="L186" s="44"/>
+      <c r="M186" s="44"/>
+      <c r="N186" s="44"/>
+      <c r="O186" s="44"/>
+      <c r="P186" s="44"/>
+      <c r="Q186" s="44"/>
+      <c r="R186" s="44"/>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
@@ -3710,20 +3799,20 @@
         <v>69</v>
       </c>
       <c r="C187" s="7"/>
-      <c r="D187" s="39"/>
-      <c r="E187" s="39"/>
-      <c r="F187" s="40"/>
-      <c r="H187" s="32"/>
-      <c r="I187" s="32"/>
-      <c r="J187" s="32"/>
-      <c r="K187" s="32"/>
-      <c r="L187" s="32"/>
-      <c r="M187" s="32"/>
-      <c r="N187" s="32"/>
-      <c r="O187" s="32"/>
-      <c r="P187" s="32"/>
-      <c r="Q187" s="32"/>
-      <c r="R187" s="32"/>
+      <c r="D187" s="47"/>
+      <c r="E187" s="47"/>
+      <c r="F187" s="48"/>
+      <c r="H187" s="44"/>
+      <c r="I187" s="44"/>
+      <c r="J187" s="44"/>
+      <c r="K187" s="44"/>
+      <c r="L187" s="44"/>
+      <c r="M187" s="44"/>
+      <c r="N187" s="44"/>
+      <c r="O187" s="44"/>
+      <c r="P187" s="44"/>
+      <c r="Q187" s="44"/>
+      <c r="R187" s="44"/>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
@@ -3733,20 +3822,20 @@
         <v>75</v>
       </c>
       <c r="C188" s="7"/>
-      <c r="D188" s="39"/>
-      <c r="E188" s="39"/>
-      <c r="F188" s="40"/>
-      <c r="H188" s="32"/>
-      <c r="I188" s="32"/>
-      <c r="J188" s="32"/>
-      <c r="K188" s="32"/>
-      <c r="L188" s="32"/>
-      <c r="M188" s="32"/>
-      <c r="N188" s="32"/>
-      <c r="O188" s="32"/>
-      <c r="P188" s="32"/>
-      <c r="Q188" s="32"/>
-      <c r="R188" s="32"/>
+      <c r="D188" s="47"/>
+      <c r="E188" s="47"/>
+      <c r="F188" s="48"/>
+      <c r="H188" s="44"/>
+      <c r="I188" s="44"/>
+      <c r="J188" s="44"/>
+      <c r="K188" s="44"/>
+      <c r="L188" s="44"/>
+      <c r="M188" s="44"/>
+      <c r="N188" s="44"/>
+      <c r="O188" s="44"/>
+      <c r="P188" s="44"/>
+      <c r="Q188" s="44"/>
+      <c r="R188" s="44"/>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
@@ -3756,22 +3845,22 @@
         <v>67</v>
       </c>
       <c r="C189" s="7" t="s">
-        <v>99</v>
-      </c>
-      <c r="D189" s="39"/>
-      <c r="E189" s="39"/>
-      <c r="F189" s="40"/>
-      <c r="H189" s="32"/>
-      <c r="I189" s="32"/>
-      <c r="J189" s="32"/>
-      <c r="K189" s="32"/>
-      <c r="L189" s="32"/>
-      <c r="M189" s="32"/>
-      <c r="N189" s="32"/>
-      <c r="O189" s="32"/>
-      <c r="P189" s="32"/>
-      <c r="Q189" s="32"/>
-      <c r="R189" s="32"/>
+        <v>98</v>
+      </c>
+      <c r="D189" s="47"/>
+      <c r="E189" s="47"/>
+      <c r="F189" s="48"/>
+      <c r="H189" s="44"/>
+      <c r="I189" s="44"/>
+      <c r="J189" s="44"/>
+      <c r="K189" s="44"/>
+      <c r="L189" s="44"/>
+      <c r="M189" s="44"/>
+      <c r="N189" s="44"/>
+      <c r="O189" s="44"/>
+      <c r="P189" s="44"/>
+      <c r="Q189" s="44"/>
+      <c r="R189" s="44"/>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
@@ -3781,20 +3870,20 @@
         <v>68</v>
       </c>
       <c r="C190" s="7"/>
-      <c r="D190" s="39"/>
-      <c r="E190" s="39"/>
-      <c r="F190" s="40"/>
-      <c r="H190" s="32"/>
-      <c r="I190" s="32"/>
-      <c r="J190" s="32"/>
-      <c r="K190" s="32"/>
-      <c r="L190" s="32"/>
-      <c r="M190" s="32"/>
-      <c r="N190" s="32"/>
-      <c r="O190" s="32"/>
-      <c r="P190" s="32"/>
-      <c r="Q190" s="32"/>
-      <c r="R190" s="32"/>
+      <c r="D190" s="47"/>
+      <c r="E190" s="47"/>
+      <c r="F190" s="48"/>
+      <c r="H190" s="44"/>
+      <c r="I190" s="44"/>
+      <c r="J190" s="44"/>
+      <c r="K190" s="44"/>
+      <c r="L190" s="44"/>
+      <c r="M190" s="44"/>
+      <c r="N190" s="44"/>
+      <c r="O190" s="44"/>
+      <c r="P190" s="44"/>
+      <c r="Q190" s="44"/>
+      <c r="R190" s="44"/>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
@@ -3804,20 +3893,20 @@
         <v>52</v>
       </c>
       <c r="C191" s="7"/>
-      <c r="D191" s="39"/>
-      <c r="E191" s="39"/>
-      <c r="F191" s="40"/>
-      <c r="H191" s="32"/>
-      <c r="I191" s="32"/>
-      <c r="J191" s="32"/>
-      <c r="K191" s="32"/>
-      <c r="L191" s="32"/>
-      <c r="M191" s="32"/>
-      <c r="N191" s="32"/>
-      <c r="O191" s="32"/>
-      <c r="P191" s="32"/>
-      <c r="Q191" s="32"/>
-      <c r="R191" s="32"/>
+      <c r="D191" s="47"/>
+      <c r="E191" s="47"/>
+      <c r="F191" s="48"/>
+      <c r="H191" s="44"/>
+      <c r="I191" s="44"/>
+      <c r="J191" s="44"/>
+      <c r="K191" s="44"/>
+      <c r="L191" s="44"/>
+      <c r="M191" s="44"/>
+      <c r="N191" s="44"/>
+      <c r="O191" s="44"/>
+      <c r="P191" s="44"/>
+      <c r="Q191" s="44"/>
+      <c r="R191" s="44"/>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
@@ -3827,20 +3916,20 @@
         <v>69</v>
       </c>
       <c r="C192" s="7"/>
-      <c r="D192" s="39"/>
-      <c r="E192" s="39"/>
-      <c r="F192" s="40"/>
-      <c r="H192" s="32"/>
-      <c r="I192" s="32"/>
-      <c r="J192" s="32"/>
-      <c r="K192" s="32"/>
-      <c r="L192" s="32"/>
-      <c r="M192" s="32"/>
-      <c r="N192" s="32"/>
-      <c r="O192" s="32"/>
-      <c r="P192" s="32"/>
-      <c r="Q192" s="32"/>
-      <c r="R192" s="32"/>
+      <c r="D192" s="47"/>
+      <c r="E192" s="47"/>
+      <c r="F192" s="48"/>
+      <c r="H192" s="44"/>
+      <c r="I192" s="44"/>
+      <c r="J192" s="44"/>
+      <c r="K192" s="44"/>
+      <c r="L192" s="44"/>
+      <c r="M192" s="44"/>
+      <c r="N192" s="44"/>
+      <c r="O192" s="44"/>
+      <c r="P192" s="44"/>
+      <c r="Q192" s="44"/>
+      <c r="R192" s="44"/>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
@@ -3850,22 +3939,22 @@
         <v>76</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D193" s="39"/>
-      <c r="E193" s="39"/>
-      <c r="F193" s="40"/>
-      <c r="H193" s="32"/>
-      <c r="I193" s="32"/>
-      <c r="J193" s="32"/>
-      <c r="K193" s="32"/>
-      <c r="L193" s="32"/>
-      <c r="M193" s="32"/>
-      <c r="N193" s="32"/>
-      <c r="O193" s="32"/>
-      <c r="P193" s="32"/>
-      <c r="Q193" s="32"/>
-      <c r="R193" s="32"/>
+        <v>99</v>
+      </c>
+      <c r="D193" s="47"/>
+      <c r="E193" s="47"/>
+      <c r="F193" s="48"/>
+      <c r="H193" s="44"/>
+      <c r="I193" s="44"/>
+      <c r="J193" s="44"/>
+      <c r="K193" s="44"/>
+      <c r="L193" s="44"/>
+      <c r="M193" s="44"/>
+      <c r="N193" s="44"/>
+      <c r="O193" s="44"/>
+      <c r="P193" s="44"/>
+      <c r="Q193" s="44"/>
+      <c r="R193" s="44"/>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
@@ -3875,22 +3964,22 @@
         <v>52</v>
       </c>
       <c r="C194" s="7" t="s">
-        <v>101</v>
-      </c>
-      <c r="D194" s="39"/>
-      <c r="E194" s="39"/>
-      <c r="F194" s="40"/>
-      <c r="H194" s="32"/>
-      <c r="I194" s="32"/>
-      <c r="J194" s="32"/>
-      <c r="K194" s="32"/>
-      <c r="L194" s="32"/>
-      <c r="M194" s="32"/>
-      <c r="N194" s="32"/>
-      <c r="O194" s="32"/>
-      <c r="P194" s="32"/>
-      <c r="Q194" s="32"/>
-      <c r="R194" s="32"/>
+        <v>100</v>
+      </c>
+      <c r="D194" s="47"/>
+      <c r="E194" s="47"/>
+      <c r="F194" s="48"/>
+      <c r="H194" s="44"/>
+      <c r="I194" s="44"/>
+      <c r="J194" s="44"/>
+      <c r="K194" s="44"/>
+      <c r="L194" s="44"/>
+      <c r="M194" s="44"/>
+      <c r="N194" s="44"/>
+      <c r="O194" s="44"/>
+      <c r="P194" s="44"/>
+      <c r="Q194" s="44"/>
+      <c r="R194" s="44"/>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
@@ -3900,20 +3989,20 @@
         <v>53</v>
       </c>
       <c r="C195" s="7"/>
-      <c r="D195" s="39"/>
-      <c r="E195" s="39"/>
-      <c r="F195" s="40"/>
-      <c r="H195" s="32"/>
-      <c r="I195" s="32"/>
-      <c r="J195" s="32"/>
-      <c r="K195" s="32"/>
-      <c r="L195" s="32"/>
-      <c r="M195" s="32"/>
-      <c r="N195" s="32"/>
-      <c r="O195" s="32"/>
-      <c r="P195" s="32"/>
-      <c r="Q195" s="32"/>
-      <c r="R195" s="32"/>
+      <c r="D195" s="47"/>
+      <c r="E195" s="47"/>
+      <c r="F195" s="48"/>
+      <c r="H195" s="44"/>
+      <c r="I195" s="44"/>
+      <c r="J195" s="44"/>
+      <c r="K195" s="44"/>
+      <c r="L195" s="44"/>
+      <c r="M195" s="44"/>
+      <c r="N195" s="44"/>
+      <c r="O195" s="44"/>
+      <c r="P195" s="44"/>
+      <c r="Q195" s="44"/>
+      <c r="R195" s="44"/>
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
@@ -3923,20 +4012,20 @@
         <v>67</v>
       </c>
       <c r="C196" s="7"/>
-      <c r="D196" s="39"/>
-      <c r="E196" s="39"/>
-      <c r="F196" s="40"/>
-      <c r="H196" s="32"/>
-      <c r="I196" s="32"/>
-      <c r="J196" s="32"/>
-      <c r="K196" s="32"/>
-      <c r="L196" s="32"/>
-      <c r="M196" s="32"/>
-      <c r="N196" s="32"/>
-      <c r="O196" s="32"/>
-      <c r="P196" s="32"/>
-      <c r="Q196" s="32"/>
-      <c r="R196" s="32"/>
+      <c r="D196" s="47"/>
+      <c r="E196" s="47"/>
+      <c r="F196" s="48"/>
+      <c r="H196" s="44"/>
+      <c r="I196" s="44"/>
+      <c r="J196" s="44"/>
+      <c r="K196" s="44"/>
+      <c r="L196" s="44"/>
+      <c r="M196" s="44"/>
+      <c r="N196" s="44"/>
+      <c r="O196" s="44"/>
+      <c r="P196" s="44"/>
+      <c r="Q196" s="44"/>
+      <c r="R196" s="44"/>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
@@ -3946,20 +4035,20 @@
         <v>69</v>
       </c>
       <c r="C197" s="7"/>
-      <c r="D197" s="39"/>
-      <c r="E197" s="39"/>
-      <c r="F197" s="40"/>
-      <c r="H197" s="32"/>
-      <c r="I197" s="32"/>
-      <c r="J197" s="32"/>
-      <c r="K197" s="32"/>
-      <c r="L197" s="32"/>
-      <c r="M197" s="32"/>
-      <c r="N197" s="32"/>
-      <c r="O197" s="32"/>
-      <c r="P197" s="32"/>
-      <c r="Q197" s="32"/>
-      <c r="R197" s="32"/>
+      <c r="D197" s="47"/>
+      <c r="E197" s="47"/>
+      <c r="F197" s="48"/>
+      <c r="H197" s="44"/>
+      <c r="I197" s="44"/>
+      <c r="J197" s="44"/>
+      <c r="K197" s="44"/>
+      <c r="L197" s="44"/>
+      <c r="M197" s="44"/>
+      <c r="N197" s="44"/>
+      <c r="O197" s="44"/>
+      <c r="P197" s="44"/>
+      <c r="Q197" s="44"/>
+      <c r="R197" s="44"/>
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
@@ -3969,11 +4058,11 @@
         <v>76</v>
       </c>
       <c r="C198" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="D198" s="39"/>
-      <c r="E198" s="39"/>
-      <c r="F198" s="40"/>
+        <v>99</v>
+      </c>
+      <c r="D198" s="47"/>
+      <c r="E198" s="47"/>
+      <c r="F198" s="48"/>
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
@@ -3983,11 +4072,11 @@
         <v>70</v>
       </c>
       <c r="C199" s="7" t="s">
-        <v>104</v>
-      </c>
-      <c r="D199" s="39"/>
-      <c r="E199" s="39"/>
-      <c r="F199" s="40"/>
+        <v>103</v>
+      </c>
+      <c r="D199" s="47"/>
+      <c r="E199" s="47"/>
+      <c r="F199" s="48"/>
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
@@ -3997,11 +4086,11 @@
         <v>71</v>
       </c>
       <c r="C200" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D200" s="39"/>
-      <c r="E200" s="39"/>
-      <c r="F200" s="40"/>
+        <v>104</v>
+      </c>
+      <c r="D200" s="47"/>
+      <c r="E200" s="47"/>
+      <c r="F200" s="48"/>
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
@@ -4011,9 +4100,9 @@
         <v>51</v>
       </c>
       <c r="C201" s="7"/>
-      <c r="D201" s="39"/>
-      <c r="E201" s="39"/>
-      <c r="F201" s="40"/>
+      <c r="D201" s="47"/>
+      <c r="E201" s="47"/>
+      <c r="F201" s="48"/>
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
@@ -4022,12 +4111,12 @@
       <c r="B202" s="6" t="s">
         <v>66</v>
       </c>
-      <c r="C202" s="28" t="s">
-        <v>106</v>
-      </c>
-      <c r="D202" s="39"/>
-      <c r="E202" s="39"/>
-      <c r="F202" s="40"/>
+      <c r="C202" s="27" t="s">
+        <v>105</v>
+      </c>
+      <c r="D202" s="47"/>
+      <c r="E202" s="47"/>
+      <c r="F202" s="48"/>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
@@ -4037,21 +4126,21 @@
         <v>78</v>
       </c>
       <c r="C203" s="7"/>
-      <c r="D203" s="39"/>
-      <c r="E203" s="39"/>
-      <c r="F203" s="40"/>
+      <c r="D203" s="47"/>
+      <c r="E203" s="47"/>
+      <c r="F203" s="48"/>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C204" s="7"/>
-      <c r="D204" s="39"/>
-      <c r="E204" s="39"/>
-      <c r="F204" s="40"/>
+      <c r="D204" s="47"/>
+      <c r="E204" s="47"/>
+      <c r="F204" s="48"/>
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
@@ -4063,9 +4152,9 @@
       <c r="C205" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="D205" s="39"/>
-      <c r="E205" s="39"/>
-      <c r="F205" s="40"/>
+      <c r="D205" s="47"/>
+      <c r="E205" s="47"/>
+      <c r="F205" s="48"/>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
@@ -4075,9 +4164,9 @@
         <v>61</v>
       </c>
       <c r="C206" s="7"/>
-      <c r="D206" s="39"/>
-      <c r="E206" s="39"/>
-      <c r="F206" s="40"/>
+      <c r="D206" s="47"/>
+      <c r="E206" s="47"/>
+      <c r="F206" s="48"/>
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
@@ -4087,9 +4176,9 @@
         <v>62</v>
       </c>
       <c r="C207" s="7"/>
-      <c r="D207" s="39"/>
-      <c r="E207" s="39"/>
-      <c r="F207" s="40"/>
+      <c r="D207" s="47"/>
+      <c r="E207" s="47"/>
+      <c r="F207" s="48"/>
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
@@ -4099,9 +4188,9 @@
         <v>32</v>
       </c>
       <c r="C208" s="7"/>
-      <c r="D208" s="39"/>
-      <c r="E208" s="39"/>
-      <c r="F208" s="40"/>
+      <c r="D208" s="47"/>
+      <c r="E208" s="47"/>
+      <c r="F208" s="48"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
@@ -4111,9 +4200,9 @@
         <v>48</v>
       </c>
       <c r="C209" s="7"/>
-      <c r="D209" s="39"/>
-      <c r="E209" s="39"/>
-      <c r="F209" s="40"/>
+      <c r="D209" s="47"/>
+      <c r="E209" s="47"/>
+      <c r="F209" s="48"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
@@ -4123,9 +4212,9 @@
         <v>63</v>
       </c>
       <c r="C210" s="7"/>
-      <c r="D210" s="39"/>
-      <c r="E210" s="39"/>
-      <c r="F210" s="40"/>
+      <c r="D210" s="47"/>
+      <c r="E210" s="47"/>
+      <c r="F210" s="48"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
@@ -4137,9 +4226,9 @@
       <c r="C211" s="7" t="s">
         <v>74</v>
       </c>
-      <c r="D211" s="39"/>
-      <c r="E211" s="39"/>
-      <c r="F211" s="40"/>
+      <c r="D211" s="47"/>
+      <c r="E211" s="47"/>
+      <c r="F211" s="48"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
@@ -4149,9 +4238,9 @@
         <v>46</v>
       </c>
       <c r="C212" s="7"/>
-      <c r="D212" s="39"/>
-      <c r="E212" s="39"/>
-      <c r="F212" s="40"/>
+      <c r="D212" s="47"/>
+      <c r="E212" s="47"/>
+      <c r="F212" s="48"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
@@ -4161,9 +4250,9 @@
         <v>40</v>
       </c>
       <c r="C213" s="7"/>
-      <c r="D213" s="39"/>
-      <c r="E213" s="39"/>
-      <c r="F213" s="40"/>
+      <c r="D213" s="47"/>
+      <c r="E213" s="47"/>
+      <c r="F213" s="48"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
@@ -4173,9 +4262,9 @@
         <v>50</v>
       </c>
       <c r="C214" s="7"/>
-      <c r="D214" s="39"/>
-      <c r="E214" s="39"/>
-      <c r="F214" s="40"/>
+      <c r="D214" s="47"/>
+      <c r="E214" s="47"/>
+      <c r="F214" s="48"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
@@ -4185,9 +4274,9 @@
         <v>69</v>
       </c>
       <c r="C215" s="7"/>
-      <c r="D215" s="39"/>
-      <c r="E215" s="39"/>
-      <c r="F215" s="40"/>
+      <c r="D215" s="47"/>
+      <c r="E215" s="47"/>
+      <c r="F215" s="48"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
@@ -4197,9 +4286,9 @@
         <v>77</v>
       </c>
       <c r="C216" s="7"/>
-      <c r="D216" s="39"/>
-      <c r="E216" s="39"/>
-      <c r="F216" s="40"/>
+      <c r="D216" s="47"/>
+      <c r="E216" s="47"/>
+      <c r="F216" s="48"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
@@ -4208,12 +4297,12 @@
       <c r="B217" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="C217" s="33" t="s">
-        <v>89</v>
-      </c>
-      <c r="D217" s="39"/>
-      <c r="E217" s="39"/>
-      <c r="F217" s="40"/>
+      <c r="C217" s="37" t="s">
+        <v>88</v>
+      </c>
+      <c r="D217" s="47"/>
+      <c r="E217" s="47"/>
+      <c r="F217" s="48"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
@@ -4222,10 +4311,10 @@
       <c r="B218" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C218" s="34"/>
-      <c r="D218" s="39"/>
-      <c r="E218" s="39"/>
-      <c r="F218" s="40"/>
+      <c r="C218" s="35"/>
+      <c r="D218" s="47"/>
+      <c r="E218" s="47"/>
+      <c r="F218" s="48"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
@@ -4234,10 +4323,10 @@
       <c r="B219" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C219" s="34"/>
-      <c r="D219" s="39"/>
-      <c r="E219" s="39"/>
-      <c r="F219" s="40"/>
+      <c r="C219" s="35"/>
+      <c r="D219" s="47"/>
+      <c r="E219" s="47"/>
+      <c r="F219" s="48"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
@@ -4246,10 +4335,10 @@
       <c r="B220" s="6" t="s">
         <v>59</v>
       </c>
-      <c r="C220" s="34"/>
-      <c r="D220" s="39"/>
-      <c r="E220" s="39"/>
-      <c r="F220" s="40"/>
+      <c r="C220" s="35"/>
+      <c r="D220" s="47"/>
+      <c r="E220" s="47"/>
+      <c r="F220" s="48"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
@@ -4258,10 +4347,10 @@
       <c r="B221" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="C221" s="34"/>
-      <c r="D221" s="39"/>
-      <c r="E221" s="39"/>
-      <c r="F221" s="40"/>
+      <c r="C221" s="35"/>
+      <c r="D221" s="47"/>
+      <c r="E221" s="47"/>
+      <c r="F221" s="48"/>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
@@ -4270,10 +4359,10 @@
       <c r="B222" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C222" s="34"/>
-      <c r="D222" s="39"/>
-      <c r="E222" s="39"/>
-      <c r="F222" s="40"/>
+      <c r="C222" s="35"/>
+      <c r="D222" s="47"/>
+      <c r="E222" s="47"/>
+      <c r="F222" s="48"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
@@ -4282,10 +4371,10 @@
       <c r="B223" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="C223" s="34"/>
-      <c r="D223" s="39"/>
-      <c r="E223" s="39"/>
-      <c r="F223" s="40"/>
+      <c r="C223" s="35"/>
+      <c r="D223" s="47"/>
+      <c r="E223" s="47"/>
+      <c r="F223" s="48"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
@@ -4294,316 +4383,418 @@
       <c r="B224" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="C224" s="35"/>
-      <c r="D224" s="39"/>
-      <c r="E224" s="39"/>
-      <c r="F224" s="40"/>
+      <c r="C224" s="36"/>
+      <c r="D224" s="47"/>
+      <c r="E224" s="47"/>
+      <c r="F224" s="48"/>
     </row>
     <row r="225" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>223</v>
       </c>
-      <c r="B225" s="8" t="s">
+      <c r="B225" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C225" s="9"/>
-      <c r="D225" s="41"/>
-      <c r="E225" s="41"/>
-      <c r="F225" s="42"/>
+      <c r="C225" s="7"/>
+      <c r="D225" s="47"/>
+      <c r="E225" s="47"/>
+      <c r="F225" s="48"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
-      <c r="B226" s="1" t="s">
+      <c r="B226" s="52" t="s">
         <v>51</v>
       </c>
-      <c r="C226" s="37" t="s">
+      <c r="C226" s="45" t="s">
         <v>80</v>
       </c>
-      <c r="D226" s="37" t="s">
+      <c r="D226" s="45" t="s">
         <v>82</v>
       </c>
-      <c r="E226" s="37"/>
-      <c r="F226" s="37"/>
+      <c r="E226" s="45"/>
+      <c r="F226" s="46"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
-      <c r="B227" s="1" t="s">
+      <c r="B227" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C227" s="32"/>
-      <c r="D227" s="32"/>
-      <c r="E227" s="32"/>
-      <c r="F227" s="32"/>
+      <c r="C227" s="47"/>
+      <c r="D227" s="47"/>
+      <c r="E227" s="47"/>
+      <c r="F227" s="48"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
-      <c r="B228" s="1" t="s">
+      <c r="B228" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C228" s="32" t="s">
+      <c r="C228" s="47" t="s">
         <v>79</v>
       </c>
-      <c r="D228" s="32"/>
-      <c r="E228" s="32"/>
-      <c r="F228" s="32"/>
+      <c r="D228" s="47"/>
+      <c r="E228" s="47"/>
+      <c r="F228" s="48"/>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
-      <c r="B229" s="1" t="s">
+      <c r="B229" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="C229" s="32"/>
-      <c r="D229" s="32"/>
-      <c r="E229" s="32"/>
-      <c r="F229" s="32"/>
+      <c r="C229" s="47"/>
+      <c r="D229" s="47"/>
+      <c r="E229" s="47"/>
+      <c r="F229" s="48"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
-      <c r="B230" s="1" t="s">
+      <c r="B230" s="6" t="s">
         <v>57</v>
       </c>
-      <c r="C230" s="32" t="s">
+      <c r="C230" s="47" t="s">
         <v>81</v>
       </c>
-      <c r="D230" s="32"/>
-      <c r="E230" s="32"/>
-      <c r="F230" s="32"/>
+      <c r="D230" s="47"/>
+      <c r="E230" s="47"/>
+      <c r="F230" s="48"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
-      <c r="B231" s="1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C231" s="32"/>
-      <c r="D231" s="32"/>
-      <c r="E231" s="32"/>
-      <c r="F231" s="32"/>
+      <c r="B231" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="C231" s="47"/>
+      <c r="D231" s="47"/>
+      <c r="E231" s="47"/>
+      <c r="F231" s="48"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
-      <c r="B232" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C232" t="s">
+      <c r="B232" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="C232" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="D232" s="32"/>
-      <c r="E232" s="32"/>
-      <c r="F232" s="32"/>
+      <c r="D232" s="47"/>
+      <c r="E232" s="47"/>
+      <c r="F232" s="48"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
-      <c r="C233" s="27" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="B233" s="6" t="s">
+        <v>134</v>
+      </c>
+      <c r="C233" s="53"/>
+      <c r="D233" s="47"/>
+      <c r="E233" s="47"/>
+      <c r="F233" s="48"/>
+    </row>
+    <row r="234" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A234" s="1">
         <v>232</v>
       </c>
+      <c r="B234" s="8"/>
+      <c r="C234" s="9"/>
+      <c r="D234" s="49"/>
+      <c r="E234" s="49"/>
+      <c r="F234" s="50"/>
     </row>
     <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
+      <c r="B235" s="1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="236" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A236" s="1">
+      <c r="A236" s="2">
         <v>234</v>
+      </c>
+      <c r="B236" s="2" t="s">
+        <v>116</v>
       </c>
     </row>
     <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
+      <c r="B237" s="1" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
+      <c r="B238" s="1" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
+      <c r="B239" s="1" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
-    </row>
-    <row r="241" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B240" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="241" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A241" s="1">
         <v>239</v>
       </c>
-    </row>
-    <row r="242" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B241" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="242" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A242" s="1">
         <v>240</v>
       </c>
-    </row>
-    <row r="243" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B242" s="1" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="243" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A243" s="1">
         <v>241</v>
       </c>
-    </row>
-    <row r="244" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B243" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="244" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A244" s="1">
         <v>242</v>
       </c>
-    </row>
-    <row r="245" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B244" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="245" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A245" s="1">
         <v>243</v>
       </c>
-    </row>
-    <row r="246" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B245" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="246" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A246" s="1">
         <v>244</v>
       </c>
-    </row>
-    <row r="247" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B246" s="1" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="247" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A247" s="1">
         <v>245</v>
       </c>
-    </row>
-    <row r="248" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B247" s="1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="248" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A248" s="1">
         <v>246</v>
       </c>
-    </row>
-    <row r="249" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B248" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="249" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A249" s="1">
         <v>247</v>
       </c>
-    </row>
-    <row r="250" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B249" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="250" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A250" s="1">
         <v>248</v>
       </c>
-    </row>
-    <row r="251" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B250" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="251" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A251" s="1">
         <v>249</v>
       </c>
-    </row>
-    <row r="252" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B251" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="252" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A252" s="1">
         <v>250</v>
       </c>
-    </row>
-    <row r="253" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B252" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="253" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A253" s="1">
         <v>251</v>
       </c>
-    </row>
-    <row r="254" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B253" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C253" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="254" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A254" s="1">
         <v>252</v>
       </c>
-    </row>
-    <row r="255" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B254" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="255" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A255" s="1">
         <v>253</v>
       </c>
-    </row>
-    <row r="256" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B255" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="256" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A256" s="1">
         <v>254</v>
       </c>
-    </row>
-    <row r="257" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B256" s="1" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A257" s="1">
         <v>255</v>
       </c>
-    </row>
-    <row r="258" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B257" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A258" s="1">
         <v>256</v>
       </c>
-    </row>
-    <row r="259" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B258" s="1" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A259" s="1">
         <v>257</v>
       </c>
-    </row>
-    <row r="260" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B259" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A260" s="1">
         <v>258</v>
       </c>
-    </row>
-    <row r="261" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B260" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A261" s="1">
         <v>259</v>
       </c>
-    </row>
-    <row r="262" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B261" s="1" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A262" s="1">
         <v>260</v>
       </c>
-    </row>
-    <row r="263" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B262" s="1" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A263" s="1">
         <v>261</v>
       </c>
-    </row>
-    <row r="264" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B263" s="1" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A264" s="1">
         <v>262</v>
       </c>
-    </row>
-    <row r="265" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B264" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A265" s="1">
         <v>263</v>
       </c>
     </row>
-    <row r="266" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A266" s="1">
         <v>264</v>
       </c>
     </row>
-    <row r="267" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A267" s="1">
         <v>265</v>
       </c>
     </row>
-    <row r="268" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A268" s="1">
         <v>266</v>
       </c>
     </row>
-    <row r="269" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A269" s="1">
         <v>267</v>
       </c>
     </row>
-    <row r="270" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A270" s="1">
         <v>268</v>
       </c>
     </row>
-    <row r="271" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A271" s="1">
         <v>269</v>
       </c>
     </row>
-    <row r="272" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A272" s="1">
         <v>270</v>
       </c>
@@ -8380,13 +8571,13 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="C2:F7"/>
-    <mergeCell ref="C8:F33"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="C52:C59"/>
-    <mergeCell ref="D34:F60"/>
+    <mergeCell ref="H177:R197"/>
+    <mergeCell ref="C217:C224"/>
+    <mergeCell ref="D169:F225"/>
+    <mergeCell ref="C226:C227"/>
+    <mergeCell ref="C228:C229"/>
+    <mergeCell ref="D226:F234"/>
     <mergeCell ref="C230:C231"/>
-    <mergeCell ref="D226:F232"/>
     <mergeCell ref="C61:C68"/>
     <mergeCell ref="C98:C105"/>
     <mergeCell ref="D61:F106"/>
@@ -8398,11 +8589,11 @@
     <mergeCell ref="D137:F168"/>
     <mergeCell ref="C128:C135"/>
     <mergeCell ref="D107:F136"/>
-    <mergeCell ref="H177:R197"/>
-    <mergeCell ref="C217:C224"/>
-    <mergeCell ref="D169:F225"/>
-    <mergeCell ref="C226:C227"/>
-    <mergeCell ref="C228:C229"/>
+    <mergeCell ref="C2:F7"/>
+    <mergeCell ref="C8:F33"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="C52:C59"/>
+    <mergeCell ref="D34:F60"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>